<commit_message>
Small update in calcSystProperties.xlsx
</commit_message>
<xml_diff>
--- a/tools/calcSystProperties.xlsx
+++ b/tools/calcSystProperties.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="145">
   <si>
     <t>Massa total</t>
   </si>
@@ -443,6 +443,15 @@
   </si>
   <si>
     <t>Displacement estimado</t>
+  </si>
+  <si>
+    <t>mean(MassDens)</t>
+  </si>
+  <si>
+    <t>Mass * Z</t>
+  </si>
+  <si>
+    <t>I roll/pitch (w.r.t own CM)</t>
   </si>
 </sst>
 </file>
@@ -633,7 +642,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -740,6 +749,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1583,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N169"/>
+  <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1597,7 +1607,7 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1644,8 +1654,8 @@
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <f>D19+D33+D57</f>
-        <v>14072252.027251249</v>
+        <f>D19+D33+D58</f>
+        <v>14072324.492717916</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -1665,7 +1675,7 @@
       </c>
       <c r="M6" s="9">
         <f>I6+M8-I7</f>
-        <v>7.4046529358542283</v>
+        <v>7.4033831622065573</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1673,8 +1683,8 @@
         <v>92</v>
       </c>
       <c r="D7" s="12">
-        <f>($D$19*D20+$D$33*D34+$D$57*D58)/$D$6</f>
-        <v>-6.3918000110561981E-3</v>
+        <f>($D$19*D20+$D$33*D34+$D$58*D59)/$D$6</f>
+        <v>-6.3917670964676468E-3</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
@@ -1684,7 +1694,7 @@
       </c>
       <c r="I7" s="9">
         <f>D26+D9</f>
-        <v>10.106987572010327</v>
+        <v>10.108257345657998</v>
       </c>
       <c r="J7" t="s">
         <v>10</v>
@@ -1695,7 +1705,7 @@
         <v>94</v>
       </c>
       <c r="D8" s="12">
-        <f>($D$19*D21+$D$33*D35+$D$57*D59)/$D$6</f>
+        <f>($D$19*D21+$D$33*D35+$D$58*D60)/$D$6</f>
         <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1724,8 +1734,8 @@
         <v>93</v>
       </c>
       <c r="D9" s="9">
-        <f>($D$19*D22+$D$33*D36+$D$57*(D32+D60))/$D$6</f>
-        <v>-9.8930124279896727</v>
+        <f>($D$19*D22+$D$33*D36+$D$58*(D32+D61))/$D$6</f>
+        <v>-9.8917426543420017</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
@@ -1755,8 +1765,8 @@
         <v>2</v>
       </c>
       <c r="D10" s="3">
-        <f>D23+$D$19*((D9-D22)^2+(D8-D21)^2)+$D$38+D61+$D$57*(($D$9-$D$56-$D$60)^2+(D8-D59)^2)</f>
-        <v>11318022819.761763</v>
+        <f>D23+$D$19*((D9-D22)^2+(D8-D21)^2)+$D$39+D62+$D$58*(($D$9-$D$57-$D$61)^2+(D8-D60)^2)</f>
+        <v>11322112687.663284</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>12</v>
@@ -1766,7 +1776,7 @@
       </c>
       <c r="I10" s="9">
         <f>I6+I8-I7</f>
-        <v>7.1941369519531673</v>
+        <v>7.1928671783054963</v>
       </c>
       <c r="J10" t="s">
         <v>10</v>
@@ -1787,8 +1797,8 @@
         <v>3</v>
       </c>
       <c r="D11" s="3">
-        <f>D24+$D$19*((D9-D22)^2+(D7-D20)^2)+$D$38+D62+$D$57*(($D$9-$D$56-$D$60)^2+(D7-D58)^2)</f>
-        <v>11303336162.377508</v>
+        <f>D24+$D$19*((D9-D22)^2+(D7-D20)^2)+$D$39+D63+$D$58*(($D$9-$D$57-$D$61)^2+(D7-D59)^2)</f>
+        <v>11307426030.279135</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>12</v>
@@ -1819,8 +1829,8 @@
         <v>4</v>
       </c>
       <c r="D12" s="3">
-        <f>D25+$D$19*((D8-D21)^2+(D7-D20))+D63+$D$57*((D8-D59)^2+(D7-D58)^2)</f>
-        <v>12283048612.905632</v>
+        <f>D25+$D$19*((D8-D21)^2+(D7-D20))+D64+$D$58*((D8-D60)^2+(D7-D59)^2)</f>
+        <v>12283048613.354862</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>12</v>
@@ -1852,7 +1862,7 @@
       </c>
       <c r="D13" s="73">
         <f>D27*B2*B3-D6*B3</f>
-        <v>1890121.862665236</v>
+        <v>1889410.9764372408</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>137</v>
@@ -1884,7 +1894,7 @@
       </c>
       <c r="D14" s="70">
         <f>D13/B3</f>
-        <v>192672.97274874983</v>
+        <v>192600.50728208365</v>
       </c>
       <c r="E14" s="67" t="s">
         <v>139</v>
@@ -2076,20 +2086,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="3:8">
+    <row r="33" spans="3:12">
       <c r="C33" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="9">
-        <f>$D$40/3 * ((D42+D52) + 4 *SUM(D43,D45,D47,D49,D51)+2*SUM(D44,D46,D48,D50))</f>
-        <v>249645.53733333331</v>
+        <f>SUM(J43:J52)</f>
+        <v>249718.00279999999</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="26"/>
     </row>
-    <row r="34" spans="3:8">
+    <row r="34" spans="3:12">
       <c r="C34" s="6" t="s">
         <v>95</v>
       </c>
@@ -2100,7 +2110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="3:8">
+    <row r="35" spans="3:12">
       <c r="C35" s="6" t="s">
         <v>97</v>
       </c>
@@ -2111,19 +2121,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="3:8">
+    <row r="36" spans="3:12">
       <c r="C36" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="9">
-        <f>$D$40/3 * ((D42*G42+D52*G52) + 4 *SUM(D43*G43,D45*G45,D47*G47,D49*G49,D51*G51)+2*SUM(D44*G44,D46*G46,D48*G48,D50*G50))/D33</f>
-        <v>43.346313798893306</v>
+        <f>SUM(L43:L52)/D33</f>
+        <v>43.402419702453265</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="3:8">
+    <row r="37" spans="3:12">
       <c r="C37" s="6" t="s">
         <v>53</v>
       </c>
@@ -2134,456 +2144,623 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="3:8">
-      <c r="C38" s="16" t="s">
+    <row r="38" spans="3:12">
+      <c r="C38" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="74">
+        <f>SUM(K43:K52)</f>
+        <v>121699827.35379744</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12">
+      <c r="C39" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="40">
-        <f>$D$40/3 * ((H42+H52) + 4 *SUM(H43,H45,H47,H49,H51)+2*SUM(H44,H46,H48,H50))</f>
-        <v>826909722.53866112</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D39" s="74">
+        <f>D33*(D36-D9)^2+D38</f>
+        <v>830965815.13161039</v>
+      </c>
+      <c r="E39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="3:8">
-      <c r="C39" s="18" t="s">
+    <row r="40" spans="3:12">
+      <c r="C40" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="3:8">
-      <c r="C40" s="14" t="s">
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="3:12">
+      <c r="C41" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="15">
-        <f>(C43-C42)*D37</f>
+      <c r="D41" s="15">
+        <f>(C44-C43)*D37</f>
         <v>7.76</v>
       </c>
-      <c r="E40" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8">
-      <c r="C41" s="14" t="s">
+      <c r="E41" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12">
+      <c r="C42" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D42" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E42" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F42" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="G42" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H42" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J42" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K42" s="16" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="42" spans="3:8">
-      <c r="C42" s="21">
+      <c r="L42" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12">
+      <c r="C43" s="21">
         <v>0</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D43" s="22">
         <v>4667</v>
       </c>
-      <c r="E42" s="22">
+      <c r="E43" s="22">
         <v>603903000000</v>
       </c>
-      <c r="F42" s="22">
+      <c r="F43" s="22">
         <v>603903000000</v>
       </c>
-      <c r="G42" s="24">
-        <f t="shared" ref="G42:G52" si="0">$D$31+C42*$D$37</f>
-        <v>10</v>
-      </c>
-      <c r="H42" s="1">
-        <f>D42*(G42-$D$9)^2</f>
-        <v>1846880.9801285276</v>
-      </c>
-    </row>
-    <row r="43" spans="3:8">
-      <c r="C43" s="21">
+      <c r="G43" s="24">
+        <f>$D$31+C43*$D$37</f>
+        <v>10</v>
+      </c>
+      <c r="H43">
+        <f>(D43+D44)/2</f>
+        <v>4506.1399999999994</v>
+      </c>
+      <c r="I43" s="9">
+        <f>(C44-C43)*$D$37</f>
+        <v>7.76</v>
+      </c>
+      <c r="J43">
+        <f>I43*H43</f>
+        <v>34967.646399999998</v>
+      </c>
+      <c r="K43" s="1">
+        <f>I43*(D43*(G43-$D$36)^2+D44*(G44-$D$36)^2)/2</f>
+        <v>31289254.644519929</v>
+      </c>
+      <c r="L43">
+        <f>J43*(G44+G43)/2</f>
+        <v>485350.93203199992</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12">
+      <c r="C44" s="21">
         <v>0.1</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D44" s="22">
         <v>4345.28</v>
       </c>
-      <c r="E43" s="22">
+      <c r="E44" s="22">
         <v>517644000000</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F44" s="22">
         <v>517644000000</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G44" s="24">
+        <f>$D$31+C44*$D$37</f>
+        <v>17.759999999999998</v>
+      </c>
+      <c r="H44">
+        <f>(D44+D45)/2</f>
+        <v>4190.0200000000004</v>
+      </c>
+      <c r="I44" s="9">
+        <f>(C45-C44)*$D$37</f>
+        <v>7.76</v>
+      </c>
+      <c r="J44">
+        <f>I44*H44</f>
+        <v>32514.555200000003</v>
+      </c>
+      <c r="K44" s="1">
+        <f>I44*(D44*(G44-$D$36)^2+D45*(G45-$D$36)^2)/2</f>
+        <v>16091940.35343617</v>
+      </c>
+      <c r="L44">
+        <f>J44*(G45+G44)/2</f>
+        <v>703614.97452800011</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12">
+      <c r="C45" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="D45" s="22">
+        <v>4034.76</v>
+      </c>
+      <c r="E45" s="22">
+        <v>440925000000</v>
+      </c>
+      <c r="F45" s="22">
+        <v>440925000000</v>
+      </c>
+      <c r="G45" s="24">
+        <f>$D$31+C45*$D$37</f>
+        <v>25.52</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ref="H45:H52" si="0">(D45+D46)/2</f>
+        <v>3885.1000000000004</v>
+      </c>
+      <c r="I45" s="9">
+        <f>(C46-C45)*$D$37</f>
+        <v>7.759999999999998</v>
+      </c>
+      <c r="J45">
+        <f>I45*H45</f>
+        <v>30148.375999999997</v>
+      </c>
+      <c r="K45" s="1">
+        <f>I45*(D45*(G45-$D$36)^2+D46*(G46-$D$36)^2)/2</f>
+        <v>6491182.317938488</v>
+      </c>
+      <c r="L45">
+        <f>J45*(G46+G45)/2</f>
+        <v>886362.25439999986</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12">
+      <c r="C46" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="D46" s="22">
+        <v>3735.44</v>
+      </c>
+      <c r="E46" s="22">
+        <v>373022000000</v>
+      </c>
+      <c r="F46" s="22">
+        <v>373022000000</v>
+      </c>
+      <c r="G46" s="24">
+        <f>$D$31+C46*$D$37</f>
+        <v>33.28</v>
+      </c>
+      <c r="H46">
         <f t="shared" si="0"/>
-        <v>17.759999999999998</v>
-      </c>
-      <c r="H43" s="1">
-        <f t="shared" ref="H43:H52" si="1">D43*(G43-$D$9)^2</f>
-        <v>3322788.2365553607</v>
-      </c>
-    </row>
-    <row r="44" spans="3:8">
-      <c r="C44" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="D44" s="22">
-        <v>4034.76</v>
-      </c>
-      <c r="E44" s="22">
-        <v>440925000000</v>
-      </c>
-      <c r="F44" s="22">
-        <v>440925000000</v>
-      </c>
-      <c r="G44" s="24">
+        <v>3591.38</v>
+      </c>
+      <c r="I46" s="9">
+        <f>(C47-C46)*$D$37</f>
+        <v>7.7600000000000025</v>
+      </c>
+      <c r="J46">
+        <f>I46*H46</f>
+        <v>27869.108800000009</v>
+      </c>
+      <c r="K46" s="1">
+        <f>I46*(D46*(G46-$D$36)^2+D47*(G47-$D$36)^2)/2</f>
+        <v>1559703.3366068501</v>
+      </c>
+      <c r="L46">
+        <f>J46*(G47+G46)/2</f>
+        <v>1035616.0830080003</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12">
+      <c r="C47" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="D47" s="22">
+        <v>3447.32</v>
+      </c>
+      <c r="E47" s="22">
+        <v>313236000000</v>
+      </c>
+      <c r="F47" s="22">
+        <v>313236000000</v>
+      </c>
+      <c r="G47" s="24">
+        <f>$D$31+C47*$D$37</f>
+        <v>41.04</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="0"/>
-        <v>25.52</v>
-      </c>
-      <c r="H44" s="1">
-        <f t="shared" si="1"/>
-        <v>5059917.668074863</v>
-      </c>
-    </row>
-    <row r="45" spans="3:8">
-      <c r="C45" s="21">
-        <v>0.3</v>
-      </c>
-      <c r="D45" s="22">
-        <v>3735.44</v>
-      </c>
-      <c r="E45" s="22">
-        <v>373022000000</v>
-      </c>
-      <c r="F45" s="22">
-        <v>373022000000</v>
-      </c>
-      <c r="G45" s="24">
+        <v>3308.86</v>
+      </c>
+      <c r="I47" s="9">
+        <f>(C48-C47)*$D$37</f>
+        <v>7.759999999999998</v>
+      </c>
+      <c r="J47">
+        <f>I47*H47</f>
+        <v>25676.753599999993</v>
+      </c>
+      <c r="K47" s="1">
+        <f>I47*(D47*(G47-$D$36)^2+D48*(G48-$D$36)^2)/2</f>
+        <v>433029.79263560765</v>
+      </c>
+      <c r="L47">
+        <f>J47*(G48+G47)/2</f>
+        <v>1153399.7717119998</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12">
+      <c r="C48" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="D48" s="22">
+        <v>3170.4</v>
+      </c>
+      <c r="E48" s="22">
+        <v>260897000000</v>
+      </c>
+      <c r="F48" s="22">
+        <v>260897000000</v>
+      </c>
+      <c r="G48" s="24">
+        <f>$D$31+C48*$D$37</f>
+        <v>48.8</v>
+      </c>
+      <c r="H48">
         <f t="shared" si="0"/>
-        <v>33.28</v>
-      </c>
-      <c r="H45" s="1">
-        <f t="shared" si="1"/>
-        <v>6962520.242831883</v>
-      </c>
-    </row>
-    <row r="46" spans="3:8">
-      <c r="C46" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="D46" s="22">
-        <v>3447.32</v>
-      </c>
-      <c r="E46" s="22">
-        <v>313236000000</v>
-      </c>
-      <c r="F46" s="22">
-        <v>313236000000</v>
-      </c>
-      <c r="G46" s="24">
+        <v>3037.5450000000001</v>
+      </c>
+      <c r="I48" s="9">
+        <f>(C49-C48)*$D$37</f>
+        <v>7.759999999999998</v>
+      </c>
+      <c r="J48">
+        <f>I48*H48</f>
+        <v>23571.349199999993</v>
+      </c>
+      <c r="K48" s="1">
+        <f>I48*(D48*(G48-$D$36)^2+D49*(G49-$D$36)^2)/2</f>
+        <v>2309498.3709639874</v>
+      </c>
+      <c r="L48">
+        <f>J48*(G49+G48)/2</f>
+        <v>1241738.6758559996</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12">
+      <c r="C49" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="D49" s="22">
+        <v>2904.69</v>
+      </c>
+      <c r="E49" s="22">
+        <v>215365000000</v>
+      </c>
+      <c r="F49" s="22">
+        <v>215365000000</v>
+      </c>
+      <c r="G49" s="24">
+        <f>$D$31+C49*$D$37</f>
+        <v>56.559999999999995</v>
+      </c>
+      <c r="H49">
         <f t="shared" si="0"/>
-        <v>41.04</v>
-      </c>
-      <c r="H46" s="1">
-        <f t="shared" si="1"/>
-        <v>8942940.1744112689</v>
-      </c>
-    </row>
-    <row r="47" spans="3:8">
-      <c r="C47" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="D47" s="22">
-        <v>3170.4</v>
-      </c>
-      <c r="E47" s="22">
-        <v>260897000000</v>
-      </c>
-      <c r="F47" s="22">
-        <v>260897000000</v>
-      </c>
-      <c r="G47" s="24">
+        <v>2777.4349999999999</v>
+      </c>
+      <c r="I49" s="9">
+        <f>(C50-C49)*$D$37</f>
+        <v>7.759999999999998</v>
+      </c>
+      <c r="J49">
+        <f>I49*H49</f>
+        <v>21552.895599999993</v>
+      </c>
+      <c r="K49" s="1">
+        <f>I49*(D49*(G49-$D$36)^2+D50*(G50-$D$36)^2)/2</f>
+        <v>6450263.1432590503</v>
+      </c>
+      <c r="L49">
+        <f>J49*(G50+G49)/2</f>
+        <v>1302657.0100639996</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12">
+      <c r="C50" s="21">
+        <v>0.7</v>
+      </c>
+      <c r="D50" s="22">
+        <v>2650.18</v>
+      </c>
+      <c r="E50" s="22">
+        <v>176028000000</v>
+      </c>
+      <c r="F50" s="22">
+        <v>176028000000</v>
+      </c>
+      <c r="G50" s="24">
+        <f>$D$31+C50*$D$37</f>
+        <v>64.319999999999993</v>
+      </c>
+      <c r="H50">
         <f t="shared" si="0"/>
-        <v>48.8</v>
-      </c>
-      <c r="H47" s="1">
-        <f t="shared" si="1"/>
-        <v>10921614.921837866</v>
-      </c>
-    </row>
-    <row r="48" spans="3:8">
-      <c r="C48" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="D48" s="22">
-        <v>2904.69</v>
-      </c>
-      <c r="E48" s="22">
-        <v>215365000000</v>
-      </c>
-      <c r="F48" s="22">
-        <v>215365000000</v>
-      </c>
-      <c r="G48" s="24">
+        <v>2528.5299999999997</v>
+      </c>
+      <c r="I50" s="9">
+        <f>(C51-C50)*$D$37</f>
+        <v>7.760000000000006</v>
+      </c>
+      <c r="J50">
+        <f>I50*H50</f>
+        <v>19621.392800000012</v>
+      </c>
+      <c r="K50" s="1">
+        <f>I50*(D50*(G50-$D$36)^2+D51*(G51-$D$36)^2)/2</f>
+        <v>12179320.976589227</v>
+      </c>
+      <c r="L50">
+        <f>J50*(G51+G50)/2</f>
+        <v>1338178.9889600007</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12">
+      <c r="C51" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="D51" s="22">
+        <v>2406.88</v>
+      </c>
+      <c r="E51" s="22">
+        <v>142301000000</v>
+      </c>
+      <c r="F51" s="22">
+        <v>142301000000</v>
+      </c>
+      <c r="G51" s="24">
+        <f>$D$31+C51*$D$37</f>
+        <v>72.08</v>
+      </c>
+      <c r="H51">
         <f t="shared" si="0"/>
-        <v>56.559999999999995</v>
-      </c>
-      <c r="H48" s="1">
-        <f t="shared" si="1"/>
-        <v>12827119.349605128</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8">
-      <c r="C49" s="21">
-        <v>0.7</v>
-      </c>
-      <c r="D49" s="22">
-        <v>2650.18</v>
-      </c>
-      <c r="E49" s="22">
-        <v>176028000000</v>
-      </c>
-      <c r="F49" s="22">
-        <v>176028000000</v>
-      </c>
-      <c r="G49" s="24">
+        <v>2290.8249999999998</v>
+      </c>
+      <c r="I51" s="9">
+        <f>(C52-C51)*$D$37</f>
+        <v>7.759999999999998</v>
+      </c>
+      <c r="J51">
+        <f>I51*H51</f>
+        <v>17776.801999999992</v>
+      </c>
+      <c r="K51" s="1">
+        <f>I51*(D51*(G51-$D$36)^2+D52*(G52-$D$36)^2)/2</f>
+        <v>18883428.326054338</v>
+      </c>
+      <c r="L51">
+        <f>J51*(G52+G51)/2</f>
+        <v>1350325.8799199995</v>
+      </c>
+    </row>
+    <row r="52" spans="3:12">
+      <c r="C52" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="D52" s="22">
+        <v>2174.77</v>
+      </c>
+      <c r="E52" s="22">
+        <v>113630000000</v>
+      </c>
+      <c r="F52" s="22">
+        <v>113630000000</v>
+      </c>
+      <c r="G52" s="24">
+        <f>$D$31+C52*$D$37</f>
+        <v>79.84</v>
+      </c>
+      <c r="H52">
         <f t="shared" si="0"/>
-        <v>64.319999999999993</v>
-      </c>
-      <c r="H49" s="1">
-        <f t="shared" si="1"/>
-        <v>14596055.078956369</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8">
-      <c r="C50" s="21">
-        <v>0.8</v>
-      </c>
-      <c r="D50" s="22">
-        <v>2406.88</v>
-      </c>
-      <c r="E50" s="22">
-        <v>142301000000</v>
-      </c>
-      <c r="F50" s="22">
-        <v>142301000000</v>
-      </c>
-      <c r="G50" s="24">
-        <f t="shared" si="0"/>
-        <v>72.08</v>
-      </c>
-      <c r="H50" s="1">
-        <f t="shared" si="1"/>
-        <v>16173210.114040092</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8">
-      <c r="C51" s="21">
-        <v>0.9</v>
-      </c>
-      <c r="D51" s="22">
-        <v>2174.77</v>
-      </c>
-      <c r="E51" s="22">
-        <v>113630000000</v>
-      </c>
-      <c r="F51" s="22">
-        <v>113630000000</v>
-      </c>
-      <c r="G51" s="24">
-        <f t="shared" si="0"/>
-        <v>79.84</v>
-      </c>
-      <c r="H51" s="1">
-        <f t="shared" si="1"/>
-        <v>17511277.441589344</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8">
-      <c r="C52" s="21">
+        <v>2064.3199999999997</v>
+      </c>
+      <c r="I52" s="9">
+        <f>(C53-C52)*$D$37</f>
+        <v>7.759999999999998</v>
+      </c>
+      <c r="J52">
+        <f>I52*H52</f>
+        <v>16019.123199999995</v>
+      </c>
+      <c r="K52" s="1">
+        <f>I52*(D52*(G52-$D$36)^2+D53*(G53-$D$36)^2)/2</f>
+        <v>26012206.091793783</v>
+      </c>
+      <c r="L52">
+        <f>J52*(G53+G52)/2</f>
+        <v>1341120.9943039995</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12">
+      <c r="C53" s="21">
         <v>1</v>
       </c>
-      <c r="D52" s="22">
+      <c r="D53" s="22">
         <v>1953.87</v>
       </c>
-      <c r="E52" s="22">
+      <c r="E53" s="22">
         <v>89488000000</v>
       </c>
-      <c r="F52" s="22">
+      <c r="F53" s="22">
         <v>89488000000</v>
       </c>
-      <c r="G52" s="24">
-        <f t="shared" si="0"/>
+      <c r="G53" s="24">
+        <f>$D$31+C53*$D$37</f>
         <v>87.6</v>
       </c>
-      <c r="H52" s="1">
-        <f t="shared" si="1"/>
-        <v>18571314.485471826</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8">
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="3:8">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="3:12">
       <c r="C54" s="6"/>
     </row>
-    <row r="55" spans="3:8" ht="18.75">
-      <c r="C55" s="8" t="s">
+    <row r="55" spans="3:12">
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="3:12" ht="18.75">
+      <c r="C56" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="3:8">
-      <c r="C56" s="6" t="s">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="3:12">
+      <c r="C57" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <f>D32</f>
         <v>87.6</v>
       </c>
-      <c r="E56" t="s">
-        <v>10</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E57" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="3:8">
-      <c r="C57" s="6" t="s">
+    <row r="58" spans="3:12">
+      <c r="C58" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="68">
-        <f>D91+D68</f>
+      <c r="D58" s="68">
+        <f>D92+D69</f>
         <v>349606.48991791578</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="3:8">
-      <c r="C58" s="6" t="s">
+    <row r="59" spans="3:12">
+      <c r="C59" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="9">
-        <f>($D$68*D69+$D$91*D95)/$D$57</f>
+      <c r="D59" s="9">
+        <f>($D$69*D70+$D$92*D96)/$D$58</f>
         <v>-0.2572807520949878</v>
       </c>
-      <c r="E58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="3:8">
-      <c r="C59" s="6" t="s">
+      <c r="E59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12">
+      <c r="C60" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D59" s="9">
-        <f>($D$68*D70+$D$91*D96)/$D$57</f>
+      <c r="D60" s="9">
+        <f>($D$69*D71+$D$92*D97)/$D$58</f>
         <v>0</v>
       </c>
-      <c r="E59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="3:8">
-      <c r="C60" s="6" t="s">
+      <c r="E60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12">
+      <c r="C61" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D60" s="9">
-        <f>($D$68*D71+$D$91*D97)/$D$57</f>
+      <c r="D61" s="9">
+        <f>($D$69*D72+$D$92*D98)/$D$58</f>
         <v>1.9532631908733569</v>
       </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="3:8">
-      <c r="C61" s="42" t="s">
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12">
+      <c r="C62" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="D61" s="43">
-        <f>D72+D98</f>
+      <c r="D62" s="43">
+        <f>D73+D99</f>
         <v>35235759.645324498</v>
-      </c>
-      <c r="E61" s="41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="3:8">
-      <c r="C62" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="43">
-        <f t="shared" ref="D62" si="2">D73+D99</f>
-        <v>20526545.746608194</v>
       </c>
       <c r="E62" s="41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="3:8">
+    <row r="63" spans="3:12">
       <c r="C63" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D63" s="43">
-        <f>D74+D100</f>
-        <v>23112723.553578477</v>
+        <f t="shared" ref="D63" si="1">D74+D100</f>
+        <v>20526545.746608194</v>
       </c>
       <c r="E63" s="41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="3:5" ht="18.75">
-      <c r="C66" s="8" t="s">
+    <row r="64" spans="3:12">
+      <c r="C64" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="43">
+        <f>D75+D101</f>
+        <v>23112723.553578477</v>
+      </c>
+      <c r="E64" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" ht="18.75">
+      <c r="C67" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="3:5">
-      <c r="C67" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D67" s="19">
-        <v>2607890</v>
-      </c>
-      <c r="E67" t="s">
-        <v>76</v>
-      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
     </row>
     <row r="68" spans="3:5">
       <c r="C68" s="6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D68" s="19">
-        <v>240000</v>
+        <v>2607890</v>
       </c>
       <c r="E68" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="3:5">
       <c r="C69" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D69" s="20">
-        <v>1.9</v>
+        <v>71</v>
+      </c>
+      <c r="D69" s="19">
+        <v>240000</v>
       </c>
       <c r="E69" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" spans="3:5">
       <c r="C70" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D70" s="20">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -2591,10 +2768,10 @@
     </row>
     <row r="71" spans="3:5">
       <c r="C71" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D71" s="20">
-        <v>1.75</v>
+        <v>0</v>
       </c>
       <c r="E71" t="s">
         <v>10</v>
@@ -2602,23 +2779,22 @@
     </row>
     <row r="72" spans="3:5">
       <c r="C72" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="1">
-        <f>D75+$D$91*(D82^2+D81^2)</f>
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="D72" s="20">
+        <v>1.75</v>
       </c>
       <c r="E72" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="3:5">
       <c r="C73" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D73" s="1">
-        <f>D76+$D$91*(D82^2+D78^2)</f>
-        <v>510093.28584317368</v>
+        <f>D76+$D$92*(D83^2+D82^2)</f>
+        <v>0</v>
       </c>
       <c r="E73" t="s">
         <v>76</v>
@@ -2626,30 +2802,31 @@
     </row>
     <row r="74" spans="3:5">
       <c r="C74" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D74" s="1">
-        <f>D77+$D$91*(D81^2+D78^2)</f>
-        <v>3117983.2858431735</v>
+        <f>D77+$D$92*(D83^2+D79^2)</f>
+        <v>510093.28584317368</v>
       </c>
       <c r="E74" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="75" spans="3:5">
-      <c r="C75" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="D75" s="49">
-        <v>0</v>
-      </c>
-      <c r="E75" s="16" t="s">
+      <c r="C75" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="1">
+        <f>D78+$D$92*(D82^2+D79^2)</f>
+        <v>3117983.2858431735</v>
+      </c>
+      <c r="E75" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="76" spans="3:5">
       <c r="C76" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D76" s="49">
         <v>0</v>
@@ -2660,11 +2837,10 @@
     </row>
     <row r="77" spans="3:5">
       <c r="C77" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D77" s="49">
-        <f>D67</f>
-        <v>2607890</v>
+        <v>0</v>
       </c>
       <c r="E77" s="16" t="s">
         <v>76</v>
@@ -2672,23 +2848,23 @@
     </row>
     <row r="78" spans="3:5">
       <c r="C78" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D78" s="24">
-        <f>D69-D58</f>
-        <v>2.1572807520949877</v>
+        <v>84</v>
+      </c>
+      <c r="D78" s="49">
+        <f>D68</f>
+        <v>2607890</v>
       </c>
       <c r="E78" s="16" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="3:5">
       <c r="C79" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D79" s="24">
-        <f t="shared" ref="D79:D80" si="3">D70-D59</f>
-        <v>0</v>
+        <f>D70-D59</f>
+        <v>2.1572807520949877</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>10</v>
@@ -2696,41 +2872,42 @@
     </row>
     <row r="80" spans="3:5">
       <c r="C80" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D80" s="24">
+        <f t="shared" ref="D80:D81" si="2">D71-D60</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5">
+      <c r="C81" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D80" s="24">
-        <f t="shared" si="3"/>
+      <c r="D81" s="24">
+        <f t="shared" si="2"/>
         <v>-0.20326319087335687</v>
       </c>
-      <c r="E80" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="3:5" ht="18.75">
-      <c r="C83" s="8" t="s">
+      <c r="E81" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" ht="18.75">
+      <c r="C84" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-    </row>
-    <row r="84" spans="3:5">
-      <c r="C84" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D84">
-        <f>D85+D111*2</f>
-        <v>126</v>
-      </c>
-      <c r="E84" t="s">
-        <v>10</v>
-      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
     </row>
     <row r="85" spans="3:5">
       <c r="C85" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D85" s="23">
-        <v>3</v>
+        <v>30</v>
+      </c>
+      <c r="D85">
+        <f>D86+D112*2</f>
+        <v>126</v>
       </c>
       <c r="E85" t="s">
         <v>10</v>
@@ -2738,11 +2915,10 @@
     </row>
     <row r="86" spans="3:5">
       <c r="C86" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D86" s="9">
-        <f>D56+D87+(-D88)*SIN(RADIANS(D89))</f>
-        <v>89.998338713738278</v>
+        <v>31</v>
+      </c>
+      <c r="D86" s="23">
+        <v>3</v>
       </c>
       <c r="E86" t="s">
         <v>10</v>
@@ -2750,10 +2926,11 @@
     </row>
     <row r="87" spans="3:5">
       <c r="C87" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D87" s="23">
-        <v>1.9625600000000001</v>
+        <v>32</v>
+      </c>
+      <c r="D87" s="9">
+        <f>D57+D88+(-D89)*SIN(RADIANS(D90))</f>
+        <v>89.998338713738278</v>
       </c>
       <c r="E87" t="s">
         <v>10</v>
@@ -2761,10 +2938,10 @@
     </row>
     <row r="88" spans="3:5">
       <c r="C88" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D88" s="23">
-        <v>-5</v>
+        <v>1.9625600000000001</v>
       </c>
       <c r="E88" t="s">
         <v>10</v>
@@ -2772,21 +2949,21 @@
     </row>
     <row r="89" spans="3:5">
       <c r="C89" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D89" s="23">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="E89" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="3:5">
       <c r="C90" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D90" s="23">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="E90" t="s">
         <v>37</v>
@@ -2794,65 +2971,65 @@
     </row>
     <row r="91" spans="3:5">
       <c r="C91" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D91" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="E91" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5">
+      <c r="C92" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D91" s="69">
-        <f>D92+D93</f>
+      <c r="D92" s="69">
+        <f>D93+D94</f>
         <v>109606.48991791575</v>
-      </c>
-    </row>
-    <row r="92" spans="3:5">
-      <c r="C92" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D92" s="34">
-        <f>D110*D112</f>
-        <v>52826.489917915751</v>
-      </c>
-      <c r="E92" s="35" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="93" spans="3:5">
       <c r="C93" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D93" s="36">
-        <v>56780</v>
+        <v>39</v>
+      </c>
+      <c r="D93" s="34">
+        <f>D111*D113</f>
+        <v>52826.489917915751</v>
       </c>
       <c r="E93" s="35" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="94" spans="3:5">
-      <c r="C94" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D94" s="44">
-        <v>115926</v>
-      </c>
-      <c r="E94" t="s">
-        <v>76</v>
+      <c r="C94" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D94" s="36">
+        <v>56780</v>
+      </c>
+      <c r="E94" s="35" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="95" spans="3:5">
       <c r="C95" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D95" s="47">
-        <f>(D88)*COS(RADIANS(D89))</f>
-        <v>-4.9809734904587275</v>
+        <v>75</v>
+      </c>
+      <c r="D95" s="44">
+        <v>115926</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="3:5">
       <c r="C96" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D96" s="47">
-        <v>0</v>
+        <f>(D89)*COS(RADIANS(D90))</f>
+        <v>-4.9809734904587275</v>
       </c>
       <c r="E96" t="s">
         <v>10</v>
@@ -2860,311 +3037,282 @@
     </row>
     <row r="97" spans="1:6">
       <c r="C97" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D97" s="47">
-        <f>D86-D56</f>
-        <v>2.3983387137382834</v>
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="C98" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D98" s="1">
-        <f>D101+$D$91*(D106^2+D105^2)</f>
-        <v>35235759.645324498</v>
-      </c>
-      <c r="E98" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="D98" s="47">
+        <f>D87-D57</f>
+        <v>2.3983387137382834</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D99" s="1">
-        <f>D102+$D$91*(D106^2+D104^2)</f>
-        <v>20016452.460765019</v>
+        <f>D102+$D$92*(D107^2+D106^2)</f>
+        <v>35235759.645324498</v>
       </c>
       <c r="E99" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="B100" s="41"/>
       <c r="C100" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D100" s="1">
-        <f>D103+$D$91*(D105^2+D104^2)</f>
-        <v>19994740.267735302</v>
+        <f>D103+$D$92*(D107^2+D105^2)</f>
+        <v>20016452.460765019</v>
       </c>
       <c r="E100" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="41"/>
       <c r="B101" s="41"/>
-      <c r="C101" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="D101" s="45">
-        <f>D94+D110*D113</f>
-        <v>35214047.452294782</v>
-      </c>
-      <c r="E101" s="35" t="s">
+      <c r="C101" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D101" s="1">
+        <f>D104+$D$92*(D106^2+D105^2)</f>
+        <v>19994740.267735302</v>
+      </c>
+      <c r="E101" t="s">
         <v>76</v>
-      </c>
-      <c r="F101" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="41"/>
       <c r="B102" s="41"/>
       <c r="C102" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D102" s="45">
-        <f>D110*D113/2</f>
-        <v>17549060.726147391</v>
+        <f>D95+D111*D114</f>
+        <v>35214047.452294782</v>
       </c>
       <c r="E102" s="35" t="s">
         <v>76</v>
       </c>
       <c r="F102" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="41"/>
       <c r="B103" s="41"/>
       <c r="C103" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D103" s="45">
-        <f>D110*D113/2</f>
+        <f>D111*D114/2</f>
         <v>17549060.726147391</v>
       </c>
       <c r="E103" s="35" t="s">
         <v>76</v>
+      </c>
+      <c r="F103" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="41"/>
       <c r="B104" s="41"/>
       <c r="C104" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D104" s="9">
-        <f>D95-D58</f>
-        <v>-4.7236927383637397</v>
+        <v>84</v>
+      </c>
+      <c r="D104" s="45">
+        <f>D111*D114/2</f>
+        <v>17549060.726147391</v>
+      </c>
+      <c r="E104" s="35" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="41"/>
       <c r="B105" s="41"/>
       <c r="C105" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D105" s="46">
+        <v>89</v>
+      </c>
+      <c r="D105" s="9">
         <f>D96-D59</f>
-        <v>0</v>
+        <v>-4.7236927383637397</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="41"/>
       <c r="B106" s="41"/>
       <c r="C106" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D106" s="46">
         <f>D97-D60</f>
-        <v>0.44507552286492658</v>
-      </c>
-      <c r="E106" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="41"/>
       <c r="B107" s="41"/>
-      <c r="C107" s="33"/>
-      <c r="D107" s="46"/>
+      <c r="C107" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D107" s="46">
+        <f>D98-D61</f>
+        <v>0.44507552286492658</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="C108" s="6"/>
-    </row>
-    <row r="109" spans="1:6" ht="18.75">
-      <c r="C109" s="8" t="s">
+      <c r="A108" s="41"/>
+      <c r="B108" s="41"/>
+      <c r="C108" s="33"/>
+      <c r="D108" s="46"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="C109" s="6"/>
+    </row>
+    <row r="110" spans="1:6" ht="18.75">
+      <c r="C110" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="C110" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D110" s="23">
-        <v>3</v>
-      </c>
-      <c r="E110" s="4"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
     </row>
     <row r="111" spans="1:6">
       <c r="C111" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D111" s="23">
-        <v>61.5</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E111" s="4"/>
     </row>
     <row r="112" spans="1:6">
       <c r="C112" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D112" s="31">
-        <f>SUM(K119:K166)</f>
-        <v>17608.829972638585</v>
+        <v>24</v>
+      </c>
+      <c r="D112" s="23">
+        <v>61.5</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F112" s="26"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="113" spans="2:13">
       <c r="C113" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113" s="31">
+        <f>SUM(K120:K167)</f>
+        <v>17608.829972638585</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="26"/>
+    </row>
+    <row r="114" spans="2:13">
+      <c r="C114" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D113" s="1">
-        <f>SUM(M119:M166)</f>
+      <c r="D114" s="1">
+        <f>SUM(M120:M167)</f>
         <v>11699373.817431593</v>
       </c>
-      <c r="E113" s="4" t="s">
+      <c r="E114" s="4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="114" spans="2:13">
-      <c r="C114" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D114" s="1">
-        <f>SUM(L119:L166)</f>
-        <v>361473.08643987949</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="115" spans="2:13">
       <c r="C115" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115" s="1">
+        <f>SUM(L120:L167)</f>
+        <v>361473.08643987949</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="2:13">
+      <c r="C116" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D115" s="9">
-        <f>D114/D112</f>
+      <c r="D116" s="9">
+        <f>D115/D113</f>
         <v>20.527944616510755</v>
       </c>
-      <c r="E115" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" spans="2:13">
-      <c r="C116" s="18" t="s">
+      <c r="E116" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="2:13">
+      <c r="C117" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="2:13">
-      <c r="C117" s="29" t="s">
+      <c r="D117" s="1"/>
+    </row>
+    <row r="118" spans="2:13">
+      <c r="C118" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="D117" s="30">
+      <c r="D118" s="30">
         <v>4.5359999999999998E-2</v>
       </c>
     </row>
-    <row r="118" spans="2:13">
-      <c r="C118" s="14" t="s">
+    <row r="119" spans="2:13">
+      <c r="C119" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D118" s="14" t="s">
+      <c r="D119" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E118" s="14" t="s">
+      <c r="E119" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F118" s="14" t="s">
+      <c r="F119" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G118" s="14" t="s">
+      <c r="G119" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H118" s="14" t="s">
+      <c r="H119" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I118" s="14" t="s">
+      <c r="I119" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="J118" s="6" t="s">
+      <c r="J119" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K118" s="14" t="s">
+      <c r="K119" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="L118" s="14" t="s">
+      <c r="L119" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="M118" s="14" t="s">
+      <c r="M119" s="14" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="119" spans="2:13">
-      <c r="C119" s="27">
-        <v>0</v>
-      </c>
-      <c r="D119" s="22">
-        <v>0.25</v>
-      </c>
-      <c r="E119" s="22">
-        <v>13.308</v>
-      </c>
-      <c r="F119" s="25">
-        <v>678.93499999999995</v>
-      </c>
-      <c r="G119" s="22">
-        <v>18110000000</v>
-      </c>
-      <c r="H119" s="22">
-        <v>18113600000</v>
-      </c>
-      <c r="I119" s="17">
-        <f t="shared" ref="I119:I166" si="4">C120-C119</f>
-        <v>3.2499999999999999E-3</v>
-      </c>
-      <c r="J119" s="16">
-        <f t="shared" ref="J119:J166" si="5">(F119+F120)/2</f>
-        <v>678.93499999999995</v>
-      </c>
-      <c r="K119" s="32">
-        <f t="shared" ref="K119:K166" si="6">I119*$D$111*J119*(1+$D$117)</f>
-        <v>141.85758188355001</v>
-      </c>
-      <c r="L119" s="1">
-        <f t="shared" ref="L119:L166" si="7">K119*((C119+C120)/2*$D$111)</f>
-        <v>14.176892089487279</v>
-      </c>
-      <c r="M119" s="1">
-        <f t="shared" ref="M119:M166" si="8">K119*((C119+C120)/2*$D$111)^2</f>
-        <v>1.4168031531931351</v>
       </c>
     </row>
     <row r="120" spans="2:13">
       <c r="C120" s="27">
-        <v>3.2499999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="D120" s="22">
         <v>0.25</v>
@@ -3182,1941 +3330,1981 @@
         <v>18113600000</v>
       </c>
       <c r="I120" s="17">
-        <f t="shared" si="4"/>
-        <v>1.626E-2</v>
+        <f t="shared" ref="I120:I167" si="3">C121-C120</f>
+        <v>3.2499999999999999E-3</v>
       </c>
       <c r="J120" s="16">
-        <f t="shared" si="5"/>
-        <v>726.149</v>
+        <f t="shared" ref="J120:J167" si="4">(F120+F121)/2</f>
+        <v>678.93499999999995</v>
       </c>
       <c r="K120" s="32">
-        <f t="shared" si="6"/>
-        <v>759.07952776881359</v>
+        <f t="shared" ref="K120:K167" si="5">I120*$D$112*J120*(1+$D$118)</f>
+        <v>141.85758188355001</v>
       </c>
       <c r="L120" s="1">
-        <f t="shared" si="7"/>
-        <v>531.25698909955952</v>
+        <f t="shared" ref="L120:L167" si="6">K120*((C120+C121)/2*$D$112)</f>
+        <v>14.176892089487279</v>
       </c>
       <c r="M120" s="1">
-        <f t="shared" si="8"/>
-        <v>371.81082896110877</v>
+        <f t="shared" ref="M120:M167" si="7">K120*((C120+C121)/2*$D$112)^2</f>
+        <v>1.4168031531931351</v>
       </c>
     </row>
     <row r="121" spans="2:13">
       <c r="C121" s="27">
-        <v>1.951E-2</v>
+        <v>3.2499999999999999E-3</v>
       </c>
       <c r="D121" s="22">
-        <v>0.25048999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="E121" s="22">
         <v>13.308</v>
       </c>
       <c r="F121" s="25">
-        <v>773.36300000000006</v>
+        <v>678.93499999999995</v>
       </c>
       <c r="G121" s="22">
-        <v>19424900000</v>
+        <v>18110000000</v>
       </c>
       <c r="H121" s="22">
-        <v>19558600000</v>
+        <v>18113600000</v>
       </c>
       <c r="I121" s="17">
+        <f t="shared" si="3"/>
+        <v>1.626E-2</v>
+      </c>
+      <c r="J121" s="16">
         <f t="shared" si="4"/>
-        <v>1.6260000000000004E-2</v>
-      </c>
-      <c r="J121" s="16">
+        <v>726.149</v>
+      </c>
+      <c r="K121" s="32">
         <f t="shared" si="5"/>
-        <v>756.95650000000001</v>
-      </c>
-      <c r="K121" s="32">
+        <v>759.07952776881359</v>
+      </c>
+      <c r="L121" s="1">
         <f t="shared" si="6"/>
-        <v>791.28413391953188</v>
-      </c>
-      <c r="L121" s="1">
+        <v>531.25698909955952</v>
+      </c>
+      <c r="M121" s="1">
         <f t="shared" si="7"/>
-        <v>1345.0722478844557</v>
-      </c>
-      <c r="M121" s="1">
-        <f t="shared" si="8"/>
-        <v>2286.4345112888709</v>
+        <v>371.81082896110877</v>
       </c>
     </row>
     <row r="122" spans="2:13">
-      <c r="B122" s="11"/>
       <c r="C122" s="27">
-        <v>3.5770000000000003E-2</v>
+        <v>1.951E-2</v>
       </c>
       <c r="D122" s="22">
-        <v>0.25490000000000002</v>
+        <v>0.25048999999999999</v>
       </c>
       <c r="E122" s="22">
         <v>13.308</v>
       </c>
       <c r="F122" s="25">
-        <v>740.55</v>
+        <v>773.36300000000006</v>
       </c>
       <c r="G122" s="22">
-        <v>17455900000</v>
+        <v>19424900000</v>
       </c>
       <c r="H122" s="22">
-        <v>19497800000</v>
+        <v>19558600000</v>
       </c>
       <c r="I122" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6260000000000004E-2</v>
+      </c>
+      <c r="J122" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J122" s="16">
+        <v>756.95650000000001</v>
+      </c>
+      <c r="K122" s="32">
         <f t="shared" si="5"/>
-        <v>740.29600000000005</v>
-      </c>
-      <c r="K122" s="32">
+        <v>791.28413391953188</v>
+      </c>
+      <c r="L122" s="1">
         <f t="shared" si="6"/>
-        <v>773.8680878017343</v>
-      </c>
-      <c r="L122" s="1">
+        <v>1345.0722478844557</v>
+      </c>
+      <c r="M122" s="1">
         <f t="shared" si="7"/>
-        <v>2089.3277568515123</v>
-      </c>
-      <c r="M122" s="1">
-        <f t="shared" si="8"/>
-        <v>5640.8715443355559</v>
+        <v>2286.4345112888709</v>
       </c>
     </row>
     <row r="123" spans="2:13">
       <c r="B123" s="11"/>
       <c r="C123" s="27">
-        <v>5.203E-2</v>
+        <v>3.5770000000000003E-2</v>
       </c>
       <c r="D123" s="22">
-        <v>0.26716000000000001</v>
+        <v>0.25490000000000002</v>
       </c>
       <c r="E123" s="22">
         <v>13.308</v>
       </c>
       <c r="F123" s="25">
-        <v>740.04200000000003</v>
+        <v>740.55</v>
       </c>
       <c r="G123" s="22">
-        <v>15287400000</v>
+        <v>17455900000</v>
       </c>
       <c r="H123" s="22">
-        <v>19788800000</v>
+        <v>19497800000</v>
       </c>
       <c r="I123" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J123" s="16">
         <f t="shared" si="4"/>
-        <v>1.6260000000000004E-2</v>
-      </c>
-      <c r="J123" s="16">
+        <v>740.29600000000005</v>
+      </c>
+      <c r="K123" s="32">
         <f t="shared" si="5"/>
-        <v>666.26900000000001</v>
-      </c>
-      <c r="K123" s="32">
+        <v>773.8680878017343</v>
+      </c>
+      <c r="L123" s="1">
         <f t="shared" si="6"/>
-        <v>696.48399693038175</v>
-      </c>
-      <c r="L123" s="1">
+        <v>2089.3277568515123</v>
+      </c>
+      <c r="M123" s="1">
         <f t="shared" si="7"/>
-        <v>2576.8793512029038</v>
-      </c>
-      <c r="M123" s="1">
-        <f t="shared" si="8"/>
-        <v>9534.0412987545533</v>
+        <v>5640.8715443355559</v>
       </c>
     </row>
     <row r="124" spans="2:13">
       <c r="B124" s="11"/>
       <c r="C124" s="27">
-        <v>6.8290000000000003E-2</v>
+        <v>5.203E-2</v>
       </c>
       <c r="D124" s="22">
-        <v>0.27940999999999999</v>
+        <v>0.26716000000000001</v>
       </c>
       <c r="E124" s="22">
         <v>13.308</v>
       </c>
       <c r="F124" s="25">
-        <v>592.49599999999998</v>
+        <v>740.04200000000003</v>
       </c>
       <c r="G124" s="22">
-        <v>10782400000</v>
+        <v>15287400000</v>
       </c>
       <c r="H124" s="22">
-        <v>14858500000</v>
+        <v>19788800000</v>
       </c>
       <c r="I124" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6260000000000004E-2</v>
+      </c>
+      <c r="J124" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J124" s="16">
+        <v>666.26900000000001</v>
+      </c>
+      <c r="K124" s="32">
         <f t="shared" si="5"/>
-        <v>521.38549999999998</v>
-      </c>
-      <c r="K124" s="32">
+        <v>696.48399693038175</v>
+      </c>
+      <c r="L124" s="1">
         <f t="shared" si="6"/>
-        <v>545.03009592453714</v>
-      </c>
-      <c r="L124" s="1">
+        <v>2576.8793512029038</v>
+      </c>
+      <c r="M124" s="1">
         <f t="shared" si="7"/>
-        <v>2561.5487957290175</v>
-      </c>
-      <c r="M124" s="1">
-        <f t="shared" si="8"/>
-        <v>12038.843876631108</v>
+        <v>9534.0412987545533</v>
       </c>
     </row>
     <row r="125" spans="2:13">
       <c r="B125" s="11"/>
       <c r="C125" s="27">
-        <v>8.455E-2</v>
+        <v>6.8290000000000003E-2</v>
       </c>
       <c r="D125" s="22">
-        <v>0.29166999999999998</v>
+        <v>0.27940999999999999</v>
       </c>
       <c r="E125" s="22">
         <v>13.308</v>
       </c>
       <c r="F125" s="25">
-        <v>450.27499999999998</v>
+        <v>592.49599999999998</v>
       </c>
       <c r="G125" s="22">
-        <v>7229720000</v>
+        <v>10782400000</v>
       </c>
       <c r="H125" s="22">
-        <v>10220600000</v>
+        <v>14858500000</v>
       </c>
       <c r="I125" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J125" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J125" s="16">
+        <v>521.38549999999998</v>
+      </c>
+      <c r="K125" s="32">
         <f t="shared" si="5"/>
-        <v>437.16449999999998</v>
-      </c>
-      <c r="K125" s="32">
+        <v>545.03009592453714</v>
+      </c>
+      <c r="L125" s="1">
         <f t="shared" si="6"/>
-        <v>456.98971177718278</v>
-      </c>
-      <c r="L125" s="1">
+        <v>2561.5487957290175</v>
+      </c>
+      <c r="M125" s="1">
         <f t="shared" si="7"/>
-        <v>2604.7590989818218</v>
-      </c>
-      <c r="M125" s="1">
-        <f t="shared" si="8"/>
-        <v>14846.658007558568</v>
+        <v>12038.843876631108</v>
       </c>
     </row>
     <row r="126" spans="2:13">
       <c r="B126" s="11"/>
       <c r="C126" s="27">
-        <v>0.10081</v>
+        <v>8.455E-2</v>
       </c>
       <c r="D126" s="22">
-        <v>0.30392000000000002</v>
+        <v>0.29166999999999998</v>
       </c>
       <c r="E126" s="22">
         <v>13.308</v>
       </c>
       <c r="F126" s="25">
-        <v>424.05399999999997</v>
+        <v>450.27499999999998</v>
       </c>
       <c r="G126" s="22">
-        <v>6309540000</v>
+        <v>7229720000</v>
       </c>
       <c r="H126" s="22">
-        <v>9144700000</v>
+        <v>10220600000</v>
       </c>
       <c r="I126" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J126" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J126" s="16">
+        <v>437.16449999999998</v>
+      </c>
+      <c r="K126" s="32">
         <f t="shared" si="5"/>
-        <v>412.346</v>
-      </c>
-      <c r="K126" s="32">
+        <v>456.98971177718278</v>
+      </c>
+      <c r="L126" s="1">
         <f t="shared" si="6"/>
-        <v>431.04570405985436</v>
-      </c>
-      <c r="L126" s="1">
+        <v>2604.7590989818218</v>
+      </c>
+      <c r="M126" s="1">
         <f t="shared" si="7"/>
-        <v>2887.9243185172527</v>
-      </c>
-      <c r="M126" s="1">
-        <f t="shared" si="8"/>
-        <v>19348.544228445069</v>
+        <v>14846.658007558568</v>
       </c>
     </row>
     <row r="127" spans="2:13">
       <c r="B127" s="11"/>
       <c r="C127" s="27">
-        <v>0.11706999999999999</v>
+        <v>0.10081</v>
       </c>
       <c r="D127" s="22">
-        <v>0.31618000000000002</v>
+        <v>0.30392000000000002</v>
       </c>
       <c r="E127" s="22">
         <v>13.308</v>
       </c>
       <c r="F127" s="25">
-        <v>400.63799999999998</v>
+        <v>424.05399999999997</v>
       </c>
       <c r="G127" s="22">
-        <v>5528360000</v>
+        <v>6309540000</v>
       </c>
       <c r="H127" s="22">
-        <v>8063160000</v>
+        <v>9144700000</v>
       </c>
       <c r="I127" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J127" s="16">
         <f t="shared" si="4"/>
-        <v>1.6280000000000003E-2</v>
-      </c>
-      <c r="J127" s="16">
+        <v>412.346</v>
+      </c>
+      <c r="K127" s="32">
         <f t="shared" si="5"/>
-        <v>391.35</v>
-      </c>
-      <c r="K127" s="32">
+        <v>431.04570405985436</v>
+      </c>
+      <c r="L127" s="1">
         <f t="shared" si="6"/>
-        <v>409.60073999592015</v>
-      </c>
-      <c r="L127" s="1">
+        <v>2887.9243185172527</v>
+      </c>
+      <c r="M127" s="1">
         <f t="shared" si="7"/>
-        <v>3154.0956822756834</v>
-      </c>
-      <c r="M127" s="1">
-        <f t="shared" si="8"/>
-        <v>24287.845703230905</v>
+        <v>19348.544228445069</v>
       </c>
     </row>
     <row r="128" spans="2:13">
       <c r="B128" s="11"/>
       <c r="C128" s="27">
-        <v>0.13335</v>
+        <v>0.11706999999999999</v>
       </c>
       <c r="D128" s="22">
-        <v>0.32844000000000001</v>
+        <v>0.31618000000000002</v>
       </c>
       <c r="E128" s="22">
         <v>13.308</v>
       </c>
       <c r="F128" s="25">
-        <v>382.06200000000001</v>
+        <v>400.63799999999998</v>
       </c>
       <c r="G128" s="22">
-        <v>4980060000</v>
+        <v>5528360000</v>
       </c>
       <c r="H128" s="22">
-        <v>6884440000</v>
+        <v>8063160000</v>
       </c>
       <c r="I128" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6280000000000003E-2</v>
+      </c>
+      <c r="J128" s="16">
         <f t="shared" si="4"/>
-        <v>1.6240000000000004E-2</v>
-      </c>
-      <c r="J128" s="16">
+        <v>391.35</v>
+      </c>
+      <c r="K128" s="32">
         <f t="shared" si="5"/>
-        <v>390.85849999999999</v>
-      </c>
-      <c r="K128" s="32">
+        <v>409.60073999592015</v>
+      </c>
+      <c r="L128" s="1">
         <f t="shared" si="6"/>
-        <v>408.08119263646574</v>
-      </c>
-      <c r="L128" s="1">
+        <v>3154.0956822756834</v>
+      </c>
+      <c r="M128" s="1">
         <f t="shared" si="7"/>
-        <v>3550.4716488202698</v>
-      </c>
-      <c r="M128" s="1">
-        <f t="shared" si="8"/>
-        <v>30890.541285754116</v>
+        <v>24287.845703230905</v>
       </c>
     </row>
     <row r="129" spans="2:13">
       <c r="B129" s="11"/>
       <c r="C129" s="27">
-        <v>0.14959</v>
+        <v>0.13335</v>
       </c>
       <c r="D129" s="22">
-        <v>0.34068999999999999</v>
+        <v>0.32844000000000001</v>
       </c>
       <c r="E129" s="22">
         <v>13.308</v>
       </c>
       <c r="F129" s="25">
-        <v>399.65499999999997</v>
+        <v>382.06200000000001</v>
       </c>
       <c r="G129" s="22">
-        <v>4936840000</v>
+        <v>4980060000</v>
       </c>
       <c r="H129" s="22">
-        <v>7009180000</v>
+        <v>6884440000</v>
       </c>
       <c r="I129" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6240000000000004E-2</v>
+      </c>
+      <c r="J129" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J129" s="16">
+        <v>390.85849999999999</v>
+      </c>
+      <c r="K129" s="32">
         <f t="shared" si="5"/>
-        <v>412.988</v>
-      </c>
-      <c r="K129" s="32">
+        <v>408.08119263646574</v>
+      </c>
+      <c r="L129" s="1">
         <f t="shared" si="6"/>
-        <v>431.71681846864317</v>
-      </c>
-      <c r="L129" s="1">
+        <v>3550.4716488202698</v>
+      </c>
+      <c r="M129" s="1">
         <f t="shared" si="7"/>
-        <v>4187.558161445776</v>
-      </c>
-      <c r="M129" s="1">
-        <f t="shared" si="8"/>
-        <v>40618.392903228509</v>
+        <v>30890.541285754116</v>
       </c>
     </row>
     <row r="130" spans="2:13">
       <c r="B130" s="11"/>
       <c r="C130" s="27">
-        <v>0.16585</v>
+        <v>0.14959</v>
       </c>
       <c r="D130" s="22">
-        <v>0.35293999999999998</v>
+        <v>0.34068999999999999</v>
       </c>
       <c r="E130" s="22">
         <v>13.308</v>
       </c>
       <c r="F130" s="25">
-        <v>426.32100000000003</v>
+        <v>399.65499999999997</v>
       </c>
       <c r="G130" s="22">
-        <v>4691660000</v>
+        <v>4936840000</v>
       </c>
       <c r="H130" s="22">
-        <v>7167680000</v>
+        <v>7009180000</v>
       </c>
       <c r="I130" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J130" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J130" s="16">
+        <v>412.988</v>
+      </c>
+      <c r="K130" s="32">
         <f t="shared" si="5"/>
-        <v>421.57050000000004</v>
-      </c>
-      <c r="K130" s="32">
+        <v>431.71681846864317</v>
+      </c>
+      <c r="L130" s="1">
         <f t="shared" si="6"/>
-        <v>440.68853095062116</v>
-      </c>
-      <c r="L130" s="1">
+        <v>4187.558161445776</v>
+      </c>
+      <c r="M130" s="1">
         <f t="shared" si="7"/>
-        <v>4715.2659228095272</v>
-      </c>
-      <c r="M130" s="1">
-        <f t="shared" si="8"/>
-        <v>50452.26086289969</v>
+        <v>40618.392903228509</v>
       </c>
     </row>
     <row r="131" spans="2:13">
       <c r="B131" s="11"/>
-      <c r="C131" s="28">
-        <v>0.18210999999999999</v>
+      <c r="C131" s="27">
+        <v>0.16585</v>
       </c>
       <c r="D131" s="22">
-        <v>0.36519000000000001</v>
+        <v>0.35293999999999998</v>
       </c>
       <c r="E131" s="22">
-        <v>13.180999999999999</v>
+        <v>13.308</v>
       </c>
       <c r="F131" s="25">
-        <v>416.82</v>
+        <v>426.32100000000003</v>
       </c>
       <c r="G131" s="22">
-        <v>3949460000</v>
+        <v>4691660000</v>
       </c>
       <c r="H131" s="22">
-        <v>7271660000</v>
+        <v>7167680000</v>
       </c>
       <c r="I131" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J131" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J131" s="16">
+        <v>421.57050000000004</v>
+      </c>
+      <c r="K131" s="32">
         <f t="shared" si="5"/>
-        <v>411.50299999999999</v>
-      </c>
-      <c r="K131" s="32">
+        <v>440.68853095062116</v>
+      </c>
+      <c r="L131" s="1">
         <f t="shared" si="6"/>
-        <v>430.16447439223913</v>
-      </c>
-      <c r="L131" s="1">
+        <v>4715.2659228095272</v>
+      </c>
+      <c r="M131" s="1">
         <f t="shared" si="7"/>
-        <v>5032.8211109153435</v>
-      </c>
-      <c r="M131" s="1">
-        <f t="shared" si="8"/>
-        <v>58882.799120642892</v>
+        <v>50452.26086289969</v>
       </c>
     </row>
     <row r="132" spans="2:13">
       <c r="B132" s="11"/>
       <c r="C132" s="28">
-        <v>0.19836999999999999</v>
+        <v>0.18210999999999999</v>
       </c>
       <c r="D132" s="22">
-        <v>0.375</v>
+        <v>0.36519000000000001</v>
       </c>
       <c r="E132" s="22">
-        <v>12.848000000000001</v>
+        <v>13.180999999999999</v>
       </c>
       <c r="F132" s="25">
-        <v>406.18599999999998</v>
+        <v>416.82</v>
       </c>
       <c r="G132" s="22">
-        <v>3386520000</v>
+        <v>3949460000</v>
       </c>
       <c r="H132" s="22">
-        <v>7081700000</v>
+        <v>7271660000</v>
       </c>
       <c r="I132" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J132" s="16">
         <f t="shared" si="4"/>
-        <v>1.6280000000000017E-2</v>
-      </c>
-      <c r="J132" s="16">
+        <v>411.50299999999999</v>
+      </c>
+      <c r="K132" s="32">
         <f t="shared" si="5"/>
-        <v>393.803</v>
-      </c>
-      <c r="K132" s="32">
+        <v>430.16447439223913</v>
+      </c>
+      <c r="L132" s="1">
         <f t="shared" si="6"/>
-        <v>412.16813648297813</v>
-      </c>
-      <c r="L132" s="1">
+        <v>5032.8211109153435</v>
+      </c>
+      <c r="M132" s="1">
         <f t="shared" si="7"/>
-        <v>5234.6857747036383</v>
-      </c>
-      <c r="M132" s="1">
-        <f t="shared" si="8"/>
-        <v>66482.419999043981</v>
+        <v>58882.799120642892</v>
       </c>
     </row>
     <row r="133" spans="2:13">
       <c r="B133" s="11"/>
       <c r="C133" s="28">
-        <v>0.21465000000000001</v>
+        <v>0.19836999999999999</v>
       </c>
       <c r="D133" s="22">
         <v>0.375</v>
       </c>
       <c r="E133" s="22">
-        <v>12.192</v>
+        <v>12.848000000000001</v>
       </c>
       <c r="F133" s="25">
-        <v>381.42</v>
+        <v>406.18599999999998</v>
       </c>
       <c r="G133" s="22">
-        <v>2933740000</v>
+        <v>3386520000</v>
       </c>
       <c r="H133" s="22">
-        <v>6244530000</v>
+        <v>7081700000</v>
       </c>
       <c r="I133" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6280000000000017E-2</v>
+      </c>
+      <c r="J133" s="16">
         <f t="shared" si="4"/>
-        <v>1.6240000000000004E-2</v>
-      </c>
-      <c r="J133" s="16">
+        <v>393.803</v>
+      </c>
+      <c r="K133" s="32">
         <f t="shared" si="5"/>
-        <v>367.12099999999998</v>
-      </c>
-      <c r="K133" s="32">
+        <v>412.16813648297813</v>
+      </c>
+      <c r="L133" s="1">
         <f t="shared" si="6"/>
-        <v>383.29772928538574</v>
-      </c>
-      <c r="L133" s="1">
+        <v>5234.6857747036383</v>
+      </c>
+      <c r="M133" s="1">
         <f t="shared" si="7"/>
-        <v>5251.3149619036813</v>
-      </c>
-      <c r="M133" s="1">
-        <f t="shared" si="8"/>
-        <v>71944.879194891924</v>
+        <v>66482.419999043981</v>
       </c>
     </row>
     <row r="134" spans="2:13">
       <c r="B134" s="11"/>
       <c r="C134" s="28">
-        <v>0.23089000000000001</v>
+        <v>0.21465000000000001</v>
       </c>
       <c r="D134" s="22">
         <v>0.375</v>
       </c>
       <c r="E134" s="22">
-        <v>11.561</v>
+        <v>12.192</v>
       </c>
       <c r="F134" s="25">
-        <v>352.822</v>
+        <v>381.42</v>
       </c>
       <c r="G134" s="22">
-        <v>2568960000</v>
+        <v>2933740000</v>
       </c>
       <c r="H134" s="22">
-        <v>5048960000</v>
+        <v>6244530000</v>
       </c>
       <c r="I134" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6240000000000004E-2</v>
+      </c>
+      <c r="J134" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999997E-2</v>
-      </c>
-      <c r="J134" s="16">
+        <v>367.12099999999998</v>
+      </c>
+      <c r="K134" s="32">
         <f t="shared" si="5"/>
-        <v>351.14949999999999</v>
-      </c>
-      <c r="K134" s="32">
+        <v>383.29772928538574</v>
+      </c>
+      <c r="L134" s="1">
         <f t="shared" si="6"/>
-        <v>367.07397054358677</v>
-      </c>
-      <c r="L134" s="1">
+        <v>5251.3149619036813</v>
+      </c>
+      <c r="M134" s="1">
         <f t="shared" si="7"/>
-        <v>5395.8882570186788</v>
-      </c>
-      <c r="M134" s="1">
-        <f t="shared" si="8"/>
-        <v>79318.100488345182</v>
+        <v>71944.879194891924</v>
       </c>
     </row>
     <row r="135" spans="2:13">
       <c r="B135" s="11"/>
       <c r="C135" s="28">
-        <v>0.24715000000000001</v>
+        <v>0.23089000000000001</v>
       </c>
       <c r="D135" s="22">
         <v>0.375</v>
       </c>
       <c r="E135" s="22">
-        <v>11.071999999999999</v>
+        <v>11.561</v>
       </c>
       <c r="F135" s="25">
-        <v>349.47699999999998</v>
+        <v>352.822</v>
       </c>
       <c r="G135" s="22">
-        <v>2388650000</v>
+        <v>2568960000</v>
       </c>
       <c r="H135" s="22">
-        <v>4948490000</v>
+        <v>5048960000</v>
       </c>
       <c r="I135" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999997E-2</v>
+      </c>
+      <c r="J135" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999969E-2</v>
-      </c>
-      <c r="J135" s="16">
+        <v>351.14949999999999</v>
+      </c>
+      <c r="K135" s="32">
         <f t="shared" si="5"/>
-        <v>348.00749999999999</v>
-      </c>
-      <c r="K135" s="32">
+        <v>367.07397054358677</v>
+      </c>
+      <c r="L135" s="1">
         <f t="shared" si="6"/>
-        <v>363.78948226879731</v>
-      </c>
-      <c r="L135" s="1">
+        <v>5395.8882570186788</v>
+      </c>
+      <c r="M135" s="1">
         <f t="shared" si="7"/>
-        <v>5711.3930105650834</v>
-      </c>
-      <c r="M135" s="1">
-        <f t="shared" si="8"/>
-        <v>89667.271075828859</v>
+        <v>79318.100488345182</v>
       </c>
     </row>
     <row r="136" spans="2:13">
       <c r="B136" s="11"/>
       <c r="C136" s="28">
-        <v>0.26340999999999998</v>
+        <v>0.24715000000000001</v>
       </c>
       <c r="D136" s="22">
         <v>0.375</v>
       </c>
       <c r="E136" s="22">
-        <v>10.792</v>
+        <v>11.071999999999999</v>
       </c>
       <c r="F136" s="25">
-        <v>346.53800000000001</v>
+        <v>349.47699999999998</v>
       </c>
       <c r="G136" s="22">
-        <v>2271990000</v>
+        <v>2388650000</v>
       </c>
       <c r="H136" s="22">
-        <v>4808020000</v>
+        <v>4948490000</v>
       </c>
       <c r="I136" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999969E-2</v>
+      </c>
+      <c r="J136" s="16">
         <f t="shared" si="4"/>
-        <v>3.2540000000000013E-2</v>
-      </c>
-      <c r="J136" s="16">
+        <v>348.00749999999999</v>
+      </c>
+      <c r="K136" s="32">
         <f t="shared" si="5"/>
-        <v>342.93550000000005</v>
-      </c>
-      <c r="K136" s="32">
+        <v>363.78948226879731</v>
+      </c>
+      <c r="L136" s="1">
         <f t="shared" si="6"/>
-        <v>717.41588273567925</v>
-      </c>
-      <c r="L136" s="1">
+        <v>5711.3930105650834</v>
+      </c>
+      <c r="M136" s="1">
         <f t="shared" si="7"/>
-        <v>12339.782756136157</v>
-      </c>
-      <c r="M136" s="1">
-        <f t="shared" si="8"/>
-        <v>212248.21213602385</v>
+        <v>89667.271075828859</v>
       </c>
     </row>
     <row r="137" spans="2:13">
       <c r="B137" s="11"/>
       <c r="C137" s="28">
-        <v>0.29594999999999999</v>
+        <v>0.26340999999999998</v>
       </c>
       <c r="D137" s="22">
         <v>0.375</v>
       </c>
       <c r="E137" s="22">
-        <v>10.231999999999999</v>
+        <v>10.792</v>
       </c>
       <c r="F137" s="25">
-        <v>339.33300000000003</v>
+        <v>346.53800000000001</v>
       </c>
       <c r="G137" s="22">
-        <v>2050050000</v>
+        <v>2271990000</v>
       </c>
       <c r="H137" s="22">
-        <v>4501400000</v>
+        <v>4808020000</v>
       </c>
       <c r="I137" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2540000000000013E-2</v>
+      </c>
+      <c r="J137" s="16">
         <f t="shared" si="4"/>
-        <v>3.2509999999999983E-2</v>
-      </c>
-      <c r="J137" s="16">
+        <v>342.93550000000005</v>
+      </c>
+      <c r="K137" s="32">
         <f t="shared" si="5"/>
-        <v>334.66849999999999</v>
-      </c>
-      <c r="K137" s="32">
+        <v>717.41588273567925</v>
+      </c>
+      <c r="L137" s="1">
         <f t="shared" si="6"/>
-        <v>699.47597216489305</v>
-      </c>
-      <c r="L137" s="1">
+        <v>12339.782756136157</v>
+      </c>
+      <c r="M137" s="1">
         <f t="shared" si="7"/>
-        <v>13430.363597219035</v>
-      </c>
-      <c r="M137" s="1">
-        <f t="shared" si="8"/>
-        <v>257871.14001249071</v>
+        <v>212248.21213602385</v>
       </c>
     </row>
     <row r="138" spans="2:13">
       <c r="B138" s="11"/>
       <c r="C138" s="28">
-        <v>0.32845999999999997</v>
+        <v>0.29594999999999999</v>
       </c>
       <c r="D138" s="22">
         <v>0.375</v>
       </c>
       <c r="E138" s="22">
-        <v>9.6720000000000006</v>
+        <v>10.231999999999999</v>
       </c>
       <c r="F138" s="25">
-        <v>330.00400000000002</v>
+        <v>339.33300000000003</v>
       </c>
       <c r="G138" s="22">
-        <v>1828250000</v>
+        <v>2050050000</v>
       </c>
       <c r="H138" s="22">
-        <v>4244070000</v>
+        <v>4501400000</v>
       </c>
       <c r="I138" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2509999999999983E-2</v>
+      </c>
+      <c r="J138" s="16">
         <f t="shared" si="4"/>
-        <v>3.2520000000000049E-2</v>
-      </c>
-      <c r="J138" s="16">
+        <v>334.66849999999999</v>
+      </c>
+      <c r="K138" s="32">
         <f t="shared" si="5"/>
-        <v>325.99700000000001</v>
-      </c>
-      <c r="K138" s="32">
+        <v>699.47597216489305</v>
+      </c>
+      <c r="L138" s="1">
         <f t="shared" si="6"/>
-        <v>681.5616321555226</v>
-      </c>
-      <c r="L138" s="1">
+        <v>13430.363597219035</v>
+      </c>
+      <c r="M138" s="1">
         <f t="shared" si="7"/>
-        <v>14449.297438954085</v>
-      </c>
-      <c r="M138" s="1">
-        <f t="shared" si="8"/>
-        <v>306329.15150910954</v>
+        <v>257871.14001249071</v>
       </c>
     </row>
     <row r="139" spans="2:13">
       <c r="B139" s="11"/>
       <c r="C139" s="28">
-        <v>0.36098000000000002</v>
+        <v>0.32845999999999997</v>
       </c>
       <c r="D139" s="22">
         <v>0.375</v>
       </c>
       <c r="E139" s="22">
-        <v>9.11</v>
+        <v>9.6720000000000006</v>
       </c>
       <c r="F139" s="25">
-        <v>321.99</v>
+        <v>330.00400000000002</v>
       </c>
       <c r="G139" s="22">
-        <v>1588710000</v>
+        <v>1828250000</v>
       </c>
       <c r="H139" s="22">
-        <v>3995280000</v>
+        <v>4244070000</v>
       </c>
       <c r="I139" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2520000000000049E-2</v>
+      </c>
+      <c r="J139" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J139" s="16">
+        <v>325.99700000000001</v>
+      </c>
+      <c r="K139" s="32">
         <f t="shared" si="5"/>
-        <v>317.90499999999997</v>
-      </c>
-      <c r="K139" s="32">
+        <v>681.5616321555226</v>
+      </c>
+      <c r="L139" s="1">
         <f t="shared" si="6"/>
-        <v>664.64369509658388</v>
-      </c>
-      <c r="L139" s="1">
+        <v>14449.297438954085</v>
+      </c>
+      <c r="M139" s="1">
         <f t="shared" si="7"/>
-        <v>15419.906533601472</v>
-      </c>
-      <c r="M139" s="1">
-        <f t="shared" si="8"/>
-        <v>357745.84075525287</v>
+        <v>306329.15150910954</v>
       </c>
     </row>
     <row r="140" spans="2:13">
       <c r="B140" s="11"/>
       <c r="C140" s="28">
-        <v>0.39350000000000002</v>
+        <v>0.36098000000000002</v>
       </c>
       <c r="D140" s="22">
         <v>0.375</v>
       </c>
       <c r="E140" s="22">
-        <v>8.5340000000000007</v>
+        <v>9.11</v>
       </c>
       <c r="F140" s="25">
-        <v>313.82</v>
+        <v>321.99</v>
       </c>
       <c r="G140" s="22">
-        <v>1361930000</v>
+        <v>1588710000</v>
       </c>
       <c r="H140" s="22">
-        <v>3750760000</v>
+        <v>3995280000</v>
       </c>
       <c r="I140" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J140" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J140" s="16">
+        <v>317.90499999999997</v>
+      </c>
+      <c r="K140" s="32">
         <f t="shared" si="5"/>
-        <v>304.27699999999999</v>
-      </c>
-      <c r="K140" s="32">
+        <v>664.64369509658388</v>
+      </c>
+      <c r="L140" s="1">
         <f t="shared" si="6"/>
-        <v>636.15164785990555</v>
-      </c>
-      <c r="L140" s="1">
+        <v>15419.906533601472</v>
+      </c>
+      <c r="M140" s="1">
         <f t="shared" si="7"/>
-        <v>16031.174202465107</v>
-      </c>
-      <c r="M140" s="1">
-        <f t="shared" si="8"/>
-        <v>403989.43738392927</v>
+        <v>357745.84075525287</v>
       </c>
     </row>
     <row r="141" spans="2:13">
       <c r="B141" s="11"/>
       <c r="C141" s="28">
-        <v>0.42602000000000001</v>
+        <v>0.39350000000000002</v>
       </c>
       <c r="D141" s="22">
         <v>0.375</v>
       </c>
       <c r="E141" s="22">
-        <v>7.9320000000000004</v>
+        <v>8.5340000000000007</v>
       </c>
       <c r="F141" s="25">
-        <v>294.73399999999998</v>
+        <v>313.82</v>
       </c>
       <c r="G141" s="22">
-        <v>1102380000</v>
+        <v>1361930000</v>
       </c>
       <c r="H141" s="22">
-        <v>3447140000</v>
+        <v>3750760000</v>
       </c>
       <c r="I141" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J141" s="16">
         <f t="shared" si="4"/>
-        <v>3.2530000000000003E-2</v>
-      </c>
-      <c r="J141" s="16">
+        <v>304.27699999999999</v>
+      </c>
+      <c r="K141" s="32">
         <f t="shared" si="5"/>
-        <v>290.92700000000002</v>
-      </c>
-      <c r="K141" s="32">
+        <v>636.15164785990555</v>
+      </c>
+      <c r="L141" s="1">
         <f t="shared" si="6"/>
-        <v>608.42785089198856</v>
-      </c>
-      <c r="L141" s="1">
+        <v>16031.174202465107</v>
+      </c>
+      <c r="M141" s="1">
         <f t="shared" si="7"/>
-        <v>16549.558489953437</v>
-      </c>
-      <c r="M141" s="1">
-        <f t="shared" si="8"/>
-        <v>450156.72081883694</v>
+        <v>403989.43738392927</v>
       </c>
     </row>
     <row r="142" spans="2:13">
       <c r="B142" s="11"/>
       <c r="C142" s="28">
-        <v>0.45855000000000001</v>
+        <v>0.42602000000000001</v>
       </c>
       <c r="D142" s="22">
         <v>0.375</v>
       </c>
       <c r="E142" s="22">
-        <v>7.3209999999999997</v>
+        <v>7.9320000000000004</v>
       </c>
       <c r="F142" s="25">
-        <v>287.12</v>
+        <v>294.73399999999998</v>
       </c>
       <c r="G142" s="22">
-        <v>875800000</v>
+        <v>1102380000</v>
       </c>
       <c r="H142" s="22">
-        <v>3139070000</v>
+        <v>3447140000</v>
       </c>
       <c r="I142" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2530000000000003E-2</v>
+      </c>
+      <c r="J142" s="16">
         <f t="shared" si="4"/>
-        <v>3.2509999999999983E-2</v>
-      </c>
-      <c r="J142" s="16">
+        <v>290.92700000000002</v>
+      </c>
+      <c r="K142" s="32">
         <f t="shared" si="5"/>
-        <v>275.23149999999998</v>
-      </c>
-      <c r="K142" s="32">
+        <v>608.42785089198856</v>
+      </c>
+      <c r="L142" s="1">
         <f t="shared" si="6"/>
-        <v>575.24930201946631</v>
-      </c>
-      <c r="L142" s="1">
+        <v>16549.558489953437</v>
+      </c>
+      <c r="M142" s="1">
         <f t="shared" si="7"/>
-        <v>16797.571557989191</v>
-      </c>
-      <c r="M142" s="1">
-        <f t="shared" si="8"/>
-        <v>490497.61426085007</v>
+        <v>450156.72081883694</v>
       </c>
     </row>
     <row r="143" spans="2:13">
       <c r="B143" s="11"/>
       <c r="C143" s="28">
-        <v>0.49106</v>
+        <v>0.45855000000000001</v>
       </c>
       <c r="D143" s="22">
         <v>0.375</v>
       </c>
       <c r="E143" s="22">
-        <v>6.7110000000000003</v>
+        <v>7.3209999999999997</v>
       </c>
       <c r="F143" s="25">
-        <v>263.34300000000002</v>
+        <v>287.12</v>
       </c>
       <c r="G143" s="22">
-        <v>681300000</v>
+        <v>875800000</v>
       </c>
       <c r="H143" s="22">
-        <v>2734240000</v>
+        <v>3139070000</v>
       </c>
       <c r="I143" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2509999999999983E-2</v>
+      </c>
+      <c r="J143" s="16">
         <f t="shared" si="4"/>
-        <v>3.2520000000000049E-2</v>
-      </c>
-      <c r="J143" s="16">
+        <v>275.23149999999998</v>
+      </c>
+      <c r="K143" s="32">
         <f t="shared" si="5"/>
-        <v>258.27499999999998</v>
-      </c>
-      <c r="K143" s="32">
+        <v>575.24930201946631</v>
+      </c>
+      <c r="L143" s="1">
         <f t="shared" si="6"/>
-        <v>539.97530819292081</v>
-      </c>
-      <c r="L143" s="1">
+        <v>16797.571557989191</v>
+      </c>
+      <c r="M143" s="1">
         <f t="shared" si="7"/>
-        <v>16847.326811174604</v>
-      </c>
-      <c r="M143" s="1">
-        <f t="shared" si="8"/>
-        <v>525639.62902747362</v>
+        <v>490497.61426085007</v>
       </c>
     </row>
     <row r="144" spans="2:13">
       <c r="B144" s="11"/>
       <c r="C144" s="28">
-        <v>0.52358000000000005</v>
+        <v>0.49106</v>
       </c>
       <c r="D144" s="22">
         <v>0.375</v>
       </c>
       <c r="E144" s="22">
-        <v>6.1219999999999999</v>
+        <v>6.7110000000000003</v>
       </c>
       <c r="F144" s="25">
-        <v>253.20699999999999</v>
+        <v>263.34300000000002</v>
       </c>
       <c r="G144" s="22">
-        <v>534720000</v>
+        <v>681300000</v>
       </c>
       <c r="H144" s="22">
-        <v>2554870000</v>
+        <v>2734240000</v>
       </c>
       <c r="I144" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2520000000000049E-2</v>
+      </c>
+      <c r="J144" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J144" s="16">
+        <v>258.27499999999998</v>
+      </c>
+      <c r="K144" s="32">
         <f t="shared" si="5"/>
-        <v>247.4365</v>
-      </c>
-      <c r="K144" s="32">
+        <v>539.97530819292081</v>
+      </c>
+      <c r="L144" s="1">
         <f t="shared" si="6"/>
-        <v>517.31526607560716</v>
-      </c>
-      <c r="L144" s="1">
+        <v>16847.326811174604</v>
+      </c>
+      <c r="M144" s="1">
         <f t="shared" si="7"/>
-        <v>17174.949604152731</v>
-      </c>
-      <c r="M144" s="1">
-        <f t="shared" si="8"/>
-        <v>570211.07484980742</v>
+        <v>525639.62902747362</v>
       </c>
     </row>
     <row r="145" spans="2:13">
       <c r="B145" s="11"/>
       <c r="C145" s="28">
-        <v>0.55610000000000004</v>
+        <v>0.52358000000000005</v>
       </c>
       <c r="D145" s="22">
         <v>0.375</v>
       </c>
       <c r="E145" s="22">
-        <v>5.5460000000000003</v>
+        <v>6.1219999999999999</v>
       </c>
       <c r="F145" s="25">
-        <v>241.666</v>
+        <v>253.20699999999999</v>
       </c>
       <c r="G145" s="22">
-        <v>408900000</v>
+        <v>534720000</v>
       </c>
       <c r="H145" s="22">
-        <v>2334030000</v>
+        <v>2554870000</v>
       </c>
       <c r="I145" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J145" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J145" s="16">
+        <v>247.4365</v>
+      </c>
+      <c r="K145" s="32">
         <f t="shared" si="5"/>
-        <v>231.15199999999999</v>
-      </c>
-      <c r="K145" s="32">
+        <v>517.31526607560716</v>
+      </c>
+      <c r="L145" s="1">
         <f t="shared" si="6"/>
-        <v>483.26927669890551</v>
-      </c>
-      <c r="L145" s="1">
+        <v>17174.949604152731</v>
+      </c>
+      <c r="M145" s="1">
         <f t="shared" si="7"/>
-        <v>17011.146197500209</v>
-      </c>
-      <c r="M145" s="1">
-        <f t="shared" si="8"/>
-        <v>598794.72771247511</v>
+        <v>570211.07484980742</v>
       </c>
     </row>
     <row r="146" spans="2:13">
       <c r="B146" s="11"/>
       <c r="C146" s="28">
-        <v>0.58862000000000003</v>
+        <v>0.55610000000000004</v>
       </c>
       <c r="D146" s="22">
         <v>0.375</v>
       </c>
       <c r="E146" s="22">
-        <v>4.9710000000000001</v>
+        <v>5.5460000000000003</v>
       </c>
       <c r="F146" s="25">
-        <v>220.63800000000001</v>
+        <v>241.666</v>
       </c>
       <c r="G146" s="22">
-        <v>314540000</v>
+        <v>408900000</v>
       </c>
       <c r="H146" s="22">
-        <v>1828730000</v>
+        <v>2334030000</v>
       </c>
       <c r="I146" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J146" s="16">
         <f t="shared" si="4"/>
-        <v>3.2529999999999948E-2</v>
-      </c>
-      <c r="J146" s="16">
+        <v>231.15199999999999</v>
+      </c>
+      <c r="K146" s="32">
         <f t="shared" si="5"/>
-        <v>210.46550000000002</v>
-      </c>
-      <c r="K146" s="32">
+        <v>483.26927669890551</v>
+      </c>
+      <c r="L146" s="1">
         <f t="shared" si="6"/>
-        <v>440.15533742797203</v>
-      </c>
-      <c r="L146" s="1">
+        <v>17011.146197500209</v>
+      </c>
+      <c r="M146" s="1">
         <f t="shared" si="7"/>
-        <v>16373.966718727312</v>
-      </c>
-      <c r="M146" s="1">
-        <f t="shared" si="8"/>
-        <v>609118.56180742825</v>
+        <v>598794.72771247511</v>
       </c>
     </row>
     <row r="147" spans="2:13">
       <c r="B147" s="11"/>
       <c r="C147" s="28">
-        <v>0.62114999999999998</v>
+        <v>0.58862000000000003</v>
       </c>
       <c r="D147" s="22">
         <v>0.375</v>
       </c>
       <c r="E147" s="22">
-        <v>4.4009999999999998</v>
+        <v>4.9710000000000001</v>
       </c>
       <c r="F147" s="25">
-        <v>200.29300000000001</v>
+        <v>220.63800000000001</v>
       </c>
       <c r="G147" s="22">
-        <v>238630000</v>
+        <v>314540000</v>
       </c>
       <c r="H147" s="22">
-        <v>1584100000</v>
+        <v>1828730000</v>
       </c>
       <c r="I147" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2529999999999948E-2</v>
+      </c>
+      <c r="J147" s="16">
         <f t="shared" si="4"/>
-        <v>3.2510000000000039E-2</v>
-      </c>
-      <c r="J147" s="16">
+        <v>210.46550000000002</v>
+      </c>
+      <c r="K147" s="32">
         <f t="shared" si="5"/>
-        <v>189.8485</v>
-      </c>
-      <c r="K147" s="32">
+        <v>440.15533742797203</v>
+      </c>
+      <c r="L147" s="1">
         <f t="shared" si="6"/>
-        <v>396.79403380224591</v>
-      </c>
-      <c r="L147" s="1">
+        <v>16373.966718727312</v>
+      </c>
+      <c r="M147" s="1">
         <f t="shared" si="7"/>
-        <v>15554.487818616813</v>
-      </c>
-      <c r="M147" s="1">
-        <f t="shared" si="8"/>
-        <v>609742.26094356505</v>
+        <v>609118.56180742825</v>
       </c>
     </row>
     <row r="148" spans="2:13">
       <c r="B148" s="11"/>
       <c r="C148" s="28">
-        <v>0.65366000000000002</v>
+        <v>0.62114999999999998</v>
       </c>
       <c r="D148" s="22">
         <v>0.375</v>
       </c>
       <c r="E148" s="22">
-        <v>3.8340000000000001</v>
+        <v>4.4009999999999998</v>
       </c>
       <c r="F148" s="25">
-        <v>179.404</v>
+        <v>200.29300000000001</v>
       </c>
       <c r="G148" s="22">
-        <v>175880000</v>
+        <v>238630000</v>
       </c>
       <c r="H148" s="22">
-        <v>1323360000</v>
+        <v>1584100000</v>
       </c>
       <c r="I148" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2510000000000039E-2</v>
+      </c>
+      <c r="J148" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J148" s="16">
+        <v>189.8485</v>
+      </c>
+      <c r="K148" s="32">
         <f t="shared" si="5"/>
-        <v>172.249</v>
-      </c>
-      <c r="K148" s="32">
+        <v>396.79403380224591</v>
+      </c>
+      <c r="L148" s="1">
         <f t="shared" si="6"/>
-        <v>360.12082803570718</v>
-      </c>
-      <c r="L148" s="1">
+        <v>15554.487818616813</v>
+      </c>
+      <c r="M148" s="1">
         <f t="shared" si="7"/>
-        <v>14837.006924737381</v>
-      </c>
-      <c r="M148" s="1">
-        <f t="shared" si="8"/>
-        <v>611285.8722597342</v>
+        <v>609742.26094356505</v>
       </c>
     </row>
     <row r="149" spans="2:13">
       <c r="B149" s="11"/>
       <c r="C149" s="28">
-        <v>0.68618000000000001</v>
+        <v>0.65366000000000002</v>
       </c>
       <c r="D149" s="22">
         <v>0.375</v>
       </c>
       <c r="E149" s="22">
-        <v>3.3319999999999999</v>
+        <v>3.8340000000000001</v>
       </c>
       <c r="F149" s="25">
-        <v>165.09399999999999</v>
+        <v>179.404</v>
       </c>
       <c r="G149" s="22">
-        <v>126010000</v>
+        <v>175880000</v>
       </c>
       <c r="H149" s="22">
-        <v>1183680000</v>
+        <v>1323360000</v>
       </c>
       <c r="I149" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J149" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J149" s="16">
+        <v>172.249</v>
+      </c>
+      <c r="K149" s="32">
         <f t="shared" si="5"/>
-        <v>159.7525</v>
-      </c>
-      <c r="K149" s="32">
+        <v>360.12082803570718</v>
+      </c>
+      <c r="L149" s="1">
         <f t="shared" si="6"/>
-        <v>333.99440682253197</v>
-      </c>
-      <c r="L149" s="1">
+        <v>14837.006924737381</v>
+      </c>
+      <c r="M149" s="1">
         <f t="shared" si="7"/>
-        <v>14428.578414397791</v>
-      </c>
-      <c r="M149" s="1">
-        <f t="shared" si="8"/>
-        <v>623315.45321668941</v>
+        <v>611285.8722597342</v>
       </c>
     </row>
     <row r="150" spans="2:13">
       <c r="B150" s="11"/>
       <c r="C150" s="28">
-        <v>0.71870000000000001</v>
+        <v>0.68618000000000001</v>
       </c>
       <c r="D150" s="22">
         <v>0.375</v>
       </c>
       <c r="E150" s="22">
-        <v>2.89</v>
+        <v>3.3319999999999999</v>
       </c>
       <c r="F150" s="25">
-        <v>154.411</v>
+        <v>165.09399999999999</v>
       </c>
       <c r="G150" s="22">
-        <v>107260000</v>
+        <v>126010000</v>
       </c>
       <c r="H150" s="22">
-        <v>1020160000</v>
+        <v>1183680000</v>
       </c>
       <c r="I150" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J150" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J150" s="16">
+        <v>159.7525</v>
+      </c>
+      <c r="K150" s="32">
         <f t="shared" si="5"/>
-        <v>146.673</v>
-      </c>
-      <c r="K150" s="32">
+        <v>333.99440682253197</v>
+      </c>
+      <c r="L150" s="1">
         <f t="shared" si="6"/>
-        <v>306.64910803825438</v>
-      </c>
-      <c r="L150" s="1">
+        <v>14428.578414397791</v>
+      </c>
+      <c r="M150" s="1">
         <f t="shared" si="7"/>
-        <v>13860.55194929342</v>
-      </c>
-      <c r="M150" s="1">
-        <f t="shared" si="8"/>
-        <v>626497.50253014057</v>
+        <v>623315.45321668941</v>
       </c>
     </row>
     <row r="151" spans="2:13">
       <c r="B151" s="11"/>
       <c r="C151" s="28">
-        <v>0.75122</v>
+        <v>0.71870000000000001</v>
       </c>
       <c r="D151" s="22">
         <v>0.375</v>
       </c>
       <c r="E151" s="22">
-        <v>2.5030000000000001</v>
+        <v>2.89</v>
       </c>
       <c r="F151" s="25">
-        <v>138.935</v>
+        <v>154.411</v>
       </c>
       <c r="G151" s="22">
-        <v>90880000</v>
+        <v>107260000</v>
       </c>
       <c r="H151" s="22">
-        <v>797810000</v>
+        <v>1020160000</v>
       </c>
       <c r="I151" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J151" s="16">
         <f t="shared" si="4"/>
-        <v>3.2540000000000013E-2</v>
-      </c>
-      <c r="J151" s="16">
+        <v>146.673</v>
+      </c>
+      <c r="K151" s="32">
         <f t="shared" si="5"/>
-        <v>134.245</v>
-      </c>
-      <c r="K151" s="32">
+        <v>306.64910803825438</v>
+      </c>
+      <c r="L151" s="1">
         <f t="shared" si="6"/>
-        <v>280.83851096737214</v>
-      </c>
-      <c r="L151" s="1">
+        <v>13860.55194929342</v>
+      </c>
+      <c r="M151" s="1">
         <f t="shared" si="7"/>
-        <v>13255.756050114429</v>
-      </c>
-      <c r="M151" s="1">
-        <f t="shared" si="8"/>
-        <v>625680.10297049279</v>
+        <v>626497.50253014057</v>
       </c>
     </row>
     <row r="152" spans="2:13">
       <c r="B152" s="11"/>
       <c r="C152" s="28">
-        <v>0.78376000000000001</v>
+        <v>0.75122</v>
       </c>
       <c r="D152" s="22">
         <v>0.375</v>
       </c>
       <c r="E152" s="22">
-        <v>2.1160000000000001</v>
+        <v>2.5030000000000001</v>
       </c>
       <c r="F152" s="25">
-        <v>129.55500000000001</v>
+        <v>138.935</v>
       </c>
       <c r="G152" s="22">
-        <v>76310000</v>
+        <v>90880000</v>
       </c>
       <c r="H152" s="22">
-        <v>709610000</v>
+        <v>797810000</v>
       </c>
       <c r="I152" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2540000000000013E-2</v>
+      </c>
+      <c r="J152" s="16">
         <f t="shared" si="4"/>
-        <v>3.2499999999999973E-2</v>
-      </c>
-      <c r="J152" s="16">
+        <v>134.245</v>
+      </c>
+      <c r="K152" s="32">
         <f t="shared" si="5"/>
-        <v>118.40950000000001</v>
-      </c>
-      <c r="K152" s="32">
+        <v>280.83851096737214</v>
+      </c>
+      <c r="L152" s="1">
         <f t="shared" si="6"/>
-        <v>247.40638414634984</v>
-      </c>
-      <c r="L152" s="1">
+        <v>13255.756050114429</v>
+      </c>
+      <c r="M152" s="1">
         <f t="shared" si="7"/>
-        <v>12172.546254926661</v>
-      </c>
-      <c r="M152" s="1">
-        <f t="shared" si="8"/>
-        <v>598896.76185833861</v>
+        <v>625680.10297049279</v>
       </c>
     </row>
     <row r="153" spans="2:13">
       <c r="B153" s="11"/>
       <c r="C153" s="28">
-        <v>0.81625999999999999</v>
+        <v>0.78376000000000001</v>
       </c>
       <c r="D153" s="22">
         <v>0.375</v>
       </c>
       <c r="E153" s="22">
-        <v>1.73</v>
+        <v>2.1160000000000001</v>
       </c>
       <c r="F153" s="25">
-        <v>107.264</v>
+        <v>129.55500000000001</v>
       </c>
       <c r="G153" s="22">
-        <v>61050000</v>
+        <v>76310000</v>
       </c>
       <c r="H153" s="22">
-        <v>518190000</v>
+        <v>709610000</v>
       </c>
       <c r="I153" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2499999999999973E-2</v>
+      </c>
+      <c r="J153" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J153" s="16">
+        <v>118.40950000000001</v>
+      </c>
+      <c r="K153" s="32">
         <f t="shared" si="5"/>
-        <v>103.02</v>
-      </c>
-      <c r="K153" s="32">
+        <v>247.40638414634984</v>
+      </c>
+      <c r="L153" s="1">
         <f t="shared" si="6"/>
-        <v>215.38382054025598</v>
-      </c>
-      <c r="L153" s="1">
+        <v>12172.546254926661</v>
+      </c>
+      <c r="M153" s="1">
         <f t="shared" si="7"/>
-        <v>11027.647303984695</v>
-      </c>
-      <c r="M153" s="1">
-        <f t="shared" si="8"/>
-        <v>564615.32141107018</v>
+        <v>598896.76185833861</v>
       </c>
     </row>
     <row r="154" spans="2:13">
       <c r="B154" s="11"/>
       <c r="C154" s="28">
-        <v>0.84877999999999998</v>
+        <v>0.81625999999999999</v>
       </c>
       <c r="D154" s="22">
         <v>0.375</v>
       </c>
       <c r="E154" s="22">
-        <v>1.3420000000000001</v>
+        <v>1.73</v>
       </c>
       <c r="F154" s="25">
-        <v>98.775999999999996</v>
+        <v>107.264</v>
       </c>
       <c r="G154" s="22">
-        <v>49480000</v>
+        <v>61050000</v>
       </c>
       <c r="H154" s="22">
-        <v>454870000</v>
+        <v>518190000</v>
       </c>
       <c r="I154" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J154" s="16">
         <f t="shared" si="4"/>
-        <v>3.2519999999999993E-2</v>
-      </c>
-      <c r="J154" s="16">
+        <v>103.02</v>
+      </c>
+      <c r="K154" s="32">
         <f t="shared" si="5"/>
-        <v>94.512</v>
-      </c>
-      <c r="K154" s="32">
+        <v>215.38382054025598</v>
+      </c>
+      <c r="L154" s="1">
         <f t="shared" si="6"/>
-        <v>197.59615265871358</v>
-      </c>
-      <c r="L154" s="1">
+        <v>11027.647303984695</v>
+      </c>
+      <c r="M154" s="1">
         <f t="shared" si="7"/>
-        <v>10512.107417597457</v>
-      </c>
-      <c r="M154" s="1">
-        <f t="shared" si="8"/>
-        <v>559243.69413188798</v>
+        <v>564615.32141107018</v>
       </c>
     </row>
     <row r="155" spans="2:13">
       <c r="B155" s="11"/>
       <c r="C155" s="28">
-        <v>0.88129999999999997</v>
+        <v>0.84877999999999998</v>
       </c>
       <c r="D155" s="22">
         <v>0.375</v>
       </c>
       <c r="E155" s="22">
-        <v>0.95399999999999996</v>
+        <v>1.3420000000000001</v>
       </c>
       <c r="F155" s="25">
-        <v>90.248000000000005</v>
+        <v>98.775999999999996</v>
       </c>
       <c r="G155" s="22">
-        <v>39360000</v>
+        <v>49480000</v>
       </c>
       <c r="H155" s="22">
-        <v>395120000</v>
+        <v>454870000</v>
       </c>
       <c r="I155" s="17">
+        <f t="shared" si="3"/>
+        <v>3.2519999999999993E-2</v>
+      </c>
+      <c r="J155" s="16">
         <f t="shared" si="4"/>
-        <v>1.6260000000000052E-2</v>
-      </c>
-      <c r="J155" s="16">
+        <v>94.512</v>
+      </c>
+      <c r="K155" s="32">
         <f t="shared" si="5"/>
-        <v>86.624500000000012</v>
-      </c>
-      <c r="K155" s="32">
+        <v>197.59615265871358</v>
+      </c>
+      <c r="L155" s="1">
         <f t="shared" si="6"/>
-        <v>90.552881782127116</v>
-      </c>
-      <c r="L155" s="1">
+        <v>10512.107417597457</v>
+      </c>
+      <c r="M155" s="1">
         <f t="shared" si="7"/>
-        <v>4953.2376530738547</v>
-      </c>
-      <c r="M155" s="1">
-        <f t="shared" si="8"/>
-        <v>270941.82719506894</v>
+        <v>559243.69413188798</v>
       </c>
     </row>
     <row r="156" spans="2:13">
       <c r="B156" s="11"/>
       <c r="C156" s="28">
-        <v>0.89756000000000002</v>
+        <v>0.88129999999999997</v>
       </c>
       <c r="D156" s="22">
         <v>0.375</v>
       </c>
       <c r="E156" s="22">
-        <v>0.76</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="F156" s="25">
-        <v>83.001000000000005</v>
+        <v>90.248000000000005</v>
       </c>
       <c r="G156" s="22">
-        <v>34670000</v>
+        <v>39360000</v>
       </c>
       <c r="H156" s="22">
-        <v>353720000</v>
+        <v>395120000</v>
       </c>
       <c r="I156" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6260000000000052E-2</v>
+      </c>
+      <c r="J156" s="16">
         <f t="shared" si="4"/>
-        <v>1.6259999999999941E-2</v>
-      </c>
-      <c r="J156" s="16">
+        <v>86.624500000000012</v>
+      </c>
+      <c r="K156" s="32">
         <f t="shared" si="5"/>
-        <v>77.953500000000005</v>
-      </c>
-      <c r="K156" s="32">
+        <v>90.552881782127116</v>
+      </c>
+      <c r="L156" s="1">
         <f t="shared" si="6"/>
-        <v>81.488655865292117</v>
-      </c>
-      <c r="L156" s="1">
+        <v>4953.2376530738547</v>
+      </c>
+      <c r="M156" s="1">
         <f t="shared" si="7"/>
-        <v>4538.912834934139</v>
-      </c>
-      <c r="M156" s="1">
-        <f t="shared" si="8"/>
-        <v>252817.14987649728</v>
+        <v>270941.82719506894</v>
       </c>
     </row>
     <row r="157" spans="2:13">
       <c r="B157" s="11"/>
       <c r="C157" s="28">
-        <v>0.91381999999999997</v>
+        <v>0.89756000000000002</v>
       </c>
       <c r="D157" s="22">
         <v>0.375</v>
       </c>
       <c r="E157" s="22">
-        <v>0.57399999999999995</v>
+        <v>0.76</v>
       </c>
       <c r="F157" s="25">
-        <v>72.906000000000006</v>
+        <v>83.001000000000005</v>
       </c>
       <c r="G157" s="22">
-        <v>30410000</v>
+        <v>34670000</v>
       </c>
       <c r="H157" s="22">
-        <v>304730000</v>
+        <v>353720000</v>
       </c>
       <c r="I157" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6259999999999941E-2</v>
+      </c>
+      <c r="J157" s="16">
         <f t="shared" si="4"/>
-        <v>1.6260000000000052E-2</v>
-      </c>
-      <c r="J157" s="16">
+        <v>77.953500000000005</v>
+      </c>
+      <c r="K157" s="32">
         <f t="shared" si="5"/>
-        <v>70.838999999999999</v>
-      </c>
-      <c r="K157" s="32">
+        <v>81.488655865292117</v>
+      </c>
+      <c r="L157" s="1">
         <f t="shared" si="6"/>
-        <v>74.051516517429846</v>
-      </c>
-      <c r="L157" s="1">
+        <v>4538.912834934139</v>
+      </c>
+      <c r="M157" s="1">
         <f t="shared" si="7"/>
-        <v>4198.7154326745331</v>
-      </c>
-      <c r="M157" s="1">
-        <f t="shared" si="8"/>
-        <v>238066.85012898859</v>
+        <v>252817.14987649728</v>
       </c>
     </row>
     <row r="158" spans="2:13">
       <c r="B158" s="11"/>
       <c r="C158" s="28">
-        <v>0.93008000000000002</v>
+        <v>0.91381999999999997</v>
       </c>
       <c r="D158" s="22">
         <v>0.375</v>
       </c>
       <c r="E158" s="22">
-        <v>0.40400000000000003</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="F158" s="25">
-        <v>68.772000000000006</v>
+        <v>72.906000000000006</v>
       </c>
       <c r="G158" s="22">
-        <v>26520000</v>
+        <v>30410000</v>
       </c>
       <c r="H158" s="22">
-        <v>281420000</v>
+        <v>304730000</v>
       </c>
       <c r="I158" s="17">
+        <f t="shared" si="3"/>
+        <v>1.6260000000000052E-2</v>
+      </c>
+      <c r="J158" s="16">
         <f t="shared" si="4"/>
-        <v>8.1299999999999706E-3</v>
-      </c>
-      <c r="J158" s="16">
+        <v>70.838999999999999</v>
+      </c>
+      <c r="K158" s="32">
         <f t="shared" si="5"/>
-        <v>67.518000000000001</v>
-      </c>
-      <c r="K158" s="32">
+        <v>74.051516517429846</v>
+      </c>
+      <c r="L158" s="1">
         <f t="shared" si="6"/>
-        <v>35.289955336917473</v>
-      </c>
-      <c r="L158" s="1">
+        <v>4198.7154326745331</v>
+      </c>
+      <c r="M158" s="1">
         <f t="shared" si="7"/>
-        <v>2027.4050226845934</v>
-      </c>
-      <c r="M158" s="1">
-        <f t="shared" si="8"/>
-        <v>116474.25129231552</v>
+        <v>238066.85012898859</v>
       </c>
     </row>
     <row r="159" spans="2:13">
       <c r="B159" s="11"/>
       <c r="C159" s="28">
-        <v>0.93820999999999999</v>
+        <v>0.93008000000000002</v>
       </c>
       <c r="D159" s="22">
         <v>0.375</v>
       </c>
       <c r="E159" s="22">
-        <v>0.31900000000000001</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="F159" s="25">
-        <v>66.263999999999996</v>
+        <v>68.772000000000006</v>
       </c>
       <c r="G159" s="22">
-        <v>23840000</v>
+        <v>26520000</v>
       </c>
       <c r="H159" s="22">
-        <v>261710000</v>
+        <v>281420000</v>
       </c>
       <c r="I159" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1299999999999706E-3</v>
+      </c>
+      <c r="J159" s="16">
         <f t="shared" si="4"/>
-        <v>8.1499999999999906E-3</v>
-      </c>
-      <c r="J159" s="16">
+        <v>67.518000000000001</v>
+      </c>
+      <c r="K159" s="32">
         <f t="shared" si="5"/>
-        <v>62.802</v>
-      </c>
-      <c r="K159" s="32">
+        <v>35.289955336917473</v>
+      </c>
+      <c r="L159" s="1">
         <f t="shared" si="6"/>
-        <v>32.905771465931956</v>
-      </c>
-      <c r="L159" s="1">
+        <v>2027.4050226845934</v>
+      </c>
+      <c r="M159" s="1">
         <f t="shared" si="7"/>
-        <v>1906.9068142452052</v>
-      </c>
-      <c r="M159" s="1">
-        <f t="shared" si="8"/>
-        <v>110506.25577885416</v>
+        <v>116474.25129231552</v>
       </c>
     </row>
     <row r="160" spans="2:13">
-      <c r="B160" s="1"/>
+      <c r="B160" s="11"/>
       <c r="C160" s="28">
-        <v>0.94635999999999998</v>
+        <v>0.93820999999999999</v>
       </c>
       <c r="D160" s="22">
         <v>0.375</v>
       </c>
       <c r="E160" s="22">
-        <v>0.253</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="F160" s="25">
-        <v>59.34</v>
+        <v>66.263999999999996</v>
       </c>
       <c r="G160" s="22">
-        <v>19630000</v>
+        <v>23840000</v>
       </c>
       <c r="H160" s="22">
-        <v>158810000</v>
+        <v>261710000</v>
       </c>
       <c r="I160" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1499999999999906E-3</v>
+      </c>
+      <c r="J160" s="16">
         <f t="shared" si="4"/>
-        <v>8.1100000000000616E-3</v>
-      </c>
-      <c r="J160" s="16">
+        <v>62.802</v>
+      </c>
+      <c r="K160" s="32">
         <f t="shared" si="5"/>
-        <v>57.627000000000002</v>
-      </c>
-      <c r="K160" s="32">
+        <v>32.905771465931956</v>
+      </c>
+      <c r="L160" s="1">
         <f t="shared" si="6"/>
-        <v>30.046082773511031</v>
-      </c>
-      <c r="L160" s="1">
+        <v>1906.9068142452052</v>
+      </c>
+      <c r="M160" s="1">
         <f t="shared" si="7"/>
-        <v>1756.2092371899689</v>
-      </c>
-      <c r="M160" s="1">
-        <f t="shared" si="8"/>
-        <v>102651.3475330801</v>
+        <v>110506.25577885416</v>
       </c>
     </row>
     <row r="161" spans="2:13">
       <c r="B161" s="1"/>
       <c r="C161" s="28">
-        <v>0.95447000000000004</v>
+        <v>0.94635999999999998</v>
       </c>
       <c r="D161" s="22">
         <v>0.375</v>
       </c>
       <c r="E161" s="22">
-        <v>0.216</v>
+        <v>0.253</v>
       </c>
       <c r="F161" s="25">
-        <v>55.914000000000001</v>
+        <v>59.34</v>
       </c>
       <c r="G161" s="22">
-        <v>16000000</v>
+        <v>19630000</v>
       </c>
       <c r="H161" s="22">
-        <v>137880000</v>
+        <v>158810000</v>
       </c>
       <c r="I161" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1100000000000616E-3</v>
+      </c>
+      <c r="J161" s="16">
         <f t="shared" si="4"/>
-        <v>8.1299999999999706E-3</v>
-      </c>
-      <c r="J161" s="16">
+        <v>57.627000000000002</v>
+      </c>
+      <c r="K161" s="32">
         <f t="shared" si="5"/>
-        <v>54.198999999999998</v>
-      </c>
-      <c r="K161" s="32">
+        <v>30.046082773511031</v>
+      </c>
+      <c r="L161" s="1">
         <f t="shared" si="6"/>
-        <v>28.328450032666698</v>
-      </c>
-      <c r="L161" s="1">
+        <v>1756.2092371899689</v>
+      </c>
+      <c r="M161" s="1">
         <f t="shared" si="7"/>
-        <v>1669.9593674018236</v>
-      </c>
-      <c r="M161" s="1">
-        <f t="shared" si="8"/>
-        <v>98443.941887299181</v>
+        <v>102651.3475330801</v>
       </c>
     </row>
     <row r="162" spans="2:13">
       <c r="B162" s="1"/>
       <c r="C162" s="28">
-        <v>0.96260000000000001</v>
+        <v>0.95447000000000004</v>
       </c>
       <c r="D162" s="22">
         <v>0.375</v>
       </c>
       <c r="E162" s="22">
-        <v>0.17799999999999999</v>
+        <v>0.216</v>
       </c>
       <c r="F162" s="25">
-        <v>52.484000000000002</v>
+        <v>55.914000000000001</v>
       </c>
       <c r="G162" s="22">
-        <v>12830000</v>
+        <v>16000000</v>
       </c>
       <c r="H162" s="22">
-        <v>118790000</v>
+        <v>137880000</v>
       </c>
       <c r="I162" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1299999999999706E-3</v>
+      </c>
+      <c r="J162" s="16">
         <f t="shared" si="4"/>
-        <v>8.1299999999999706E-3</v>
-      </c>
-      <c r="J162" s="16">
+        <v>54.198999999999998</v>
+      </c>
+      <c r="K162" s="32">
         <f t="shared" si="5"/>
-        <v>50.798999999999999</v>
-      </c>
-      <c r="K162" s="32">
+        <v>28.328450032666698</v>
+      </c>
+      <c r="L162" s="1">
         <f t="shared" si="6"/>
-        <v>26.551355803786706</v>
-      </c>
-      <c r="L162" s="1">
+        <v>1669.9593674018236</v>
+      </c>
+      <c r="M162" s="1">
         <f t="shared" si="7"/>
-        <v>1578.4753810211498</v>
-      </c>
-      <c r="M162" s="1">
-        <f t="shared" si="8"/>
-        <v>93840.199607980787</v>
+        <v>98443.941887299181</v>
       </c>
     </row>
     <row r="163" spans="2:13">
       <c r="B163" s="1"/>
       <c r="C163" s="28">
-        <v>0.97072999999999998</v>
+        <v>0.96260000000000001</v>
       </c>
       <c r="D163" s="22">
         <v>0.375</v>
       </c>
       <c r="E163" s="22">
-        <v>0.14000000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="F163" s="25">
-        <v>49.113999999999997</v>
+        <v>52.484000000000002</v>
       </c>
       <c r="G163" s="22">
-        <v>10080000</v>
+        <v>12830000</v>
       </c>
       <c r="H163" s="22">
-        <v>101630000</v>
+        <v>118790000</v>
       </c>
       <c r="I163" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1299999999999706E-3</v>
+      </c>
+      <c r="J163" s="16">
         <f t="shared" si="4"/>
-        <v>8.1299999999999706E-3</v>
-      </c>
-      <c r="J163" s="16">
+        <v>50.798999999999999</v>
+      </c>
+      <c r="K163" s="32">
         <f t="shared" si="5"/>
-        <v>47.465999999999994</v>
-      </c>
-      <c r="K163" s="32">
+        <v>26.551355803786706</v>
+      </c>
+      <c r="L163" s="1">
         <f t="shared" si="6"/>
-        <v>24.80928078471111</v>
-      </c>
-      <c r="L163" s="1">
+        <v>1578.4753810211498</v>
+      </c>
+      <c r="M163" s="1">
         <f t="shared" si="7"/>
-        <v>1487.3137160457466</v>
-      </c>
-      <c r="M163" s="1">
-        <f t="shared" si="8"/>
-        <v>89164.297390718028</v>
+        <v>93840.199607980787</v>
       </c>
     </row>
     <row r="164" spans="2:13">
       <c r="B164" s="1"/>
       <c r="C164" s="28">
-        <v>0.97885999999999995</v>
+        <v>0.97072999999999998</v>
       </c>
       <c r="D164" s="22">
         <v>0.375</v>
       </c>
       <c r="E164" s="22">
-        <v>0.10100000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F164" s="25">
-        <v>45.817999999999998</v>
+        <v>49.113999999999997</v>
       </c>
       <c r="G164" s="22">
-        <v>7550000</v>
+        <v>10080000</v>
       </c>
       <c r="H164" s="22">
-        <v>85070000</v>
+        <v>101630000</v>
       </c>
       <c r="I164" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1299999999999706E-3</v>
+      </c>
+      <c r="J164" s="16">
         <f t="shared" si="4"/>
-        <v>8.1300000000000816E-3</v>
-      </c>
-      <c r="J164" s="16">
+        <v>47.465999999999994</v>
+      </c>
+      <c r="K164" s="32">
         <f t="shared" si="5"/>
-        <v>43.743499999999997</v>
-      </c>
-      <c r="K164" s="32">
+        <v>24.80928078471111</v>
+      </c>
+      <c r="L164" s="1">
         <f t="shared" si="6"/>
-        <v>22.86362394147443</v>
-      </c>
-      <c r="L164" s="1">
+        <v>1487.3137160457466</v>
+      </c>
+      <c r="M164" s="1">
         <f t="shared" si="7"/>
-        <v>1382.103495104436</v>
-      </c>
-      <c r="M164" s="1">
-        <f t="shared" si="8"/>
-        <v>83548.00079241996</v>
+        <v>89164.297390718028</v>
       </c>
     </row>
     <row r="165" spans="2:13">
       <c r="B165" s="1"/>
       <c r="C165" s="28">
-        <v>0.98699000000000003</v>
+        <v>0.97885999999999995</v>
       </c>
       <c r="D165" s="22">
         <v>0.375</v>
       </c>
       <c r="E165" s="22">
-        <v>6.2E-2</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="F165" s="25">
-        <v>41.668999999999997</v>
+        <v>45.817999999999998</v>
       </c>
       <c r="G165" s="22">
-        <v>4600000</v>
+        <v>7550000</v>
       </c>
       <c r="H165" s="22">
-        <v>64260000</v>
+        <v>85070000</v>
       </c>
       <c r="I165" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1300000000000816E-3</v>
+      </c>
+      <c r="J165" s="16">
         <f t="shared" si="4"/>
-        <v>8.1299999999999706E-3</v>
-      </c>
-      <c r="J165" s="16">
+        <v>43.743499999999997</v>
+      </c>
+      <c r="K165" s="32">
         <f t="shared" si="5"/>
-        <v>26.561</v>
-      </c>
-      <c r="K165" s="32">
+        <v>22.86362394147443</v>
+      </c>
+      <c r="L165" s="1">
         <f t="shared" si="6"/>
-        <v>13.88276465096515</v>
-      </c>
-      <c r="L165" s="1">
+        <v>1382.103495104436</v>
+      </c>
+      <c r="M165" s="1">
         <f t="shared" si="7"/>
-        <v>846.15287425147937</v>
-      </c>
-      <c r="M165" s="1">
-        <f t="shared" si="8"/>
-        <v>51572.918262664949</v>
+        <v>83548.00079241996</v>
       </c>
     </row>
     <row r="166" spans="2:13">
       <c r="B166" s="1"/>
       <c r="C166" s="28">
-        <v>0.99512</v>
+        <v>0.98699000000000003</v>
       </c>
       <c r="D166" s="22">
         <v>0.375</v>
       </c>
       <c r="E166" s="22">
-        <v>2.3E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="F166" s="25">
-        <v>11.452999999999999</v>
+        <v>41.668999999999997</v>
       </c>
       <c r="G166" s="22">
-        <v>250000</v>
+        <v>4600000</v>
       </c>
       <c r="H166" s="22">
-        <v>6610000</v>
+        <v>64260000</v>
       </c>
       <c r="I166" s="17">
+        <f t="shared" si="3"/>
+        <v>8.1299999999999706E-3</v>
+      </c>
+      <c r="J166" s="16">
         <f t="shared" si="4"/>
-        <v>4.8799999999999955E-3</v>
-      </c>
-      <c r="J166" s="16">
+        <v>26.561</v>
+      </c>
+      <c r="K166" s="32">
         <f t="shared" si="5"/>
-        <v>10.885999999999999</v>
-      </c>
-      <c r="K166" s="32">
+        <v>13.88276465096515</v>
+      </c>
+      <c r="L166" s="1">
         <f t="shared" si="6"/>
-        <v>3.4153022626751968</v>
-      </c>
-      <c r="L166" s="1">
+        <v>846.15287425147937</v>
+      </c>
+      <c r="M166" s="1">
         <f t="shared" si="7"/>
-        <v>209.52858889698757</v>
-      </c>
-      <c r="M166" s="1">
-        <f t="shared" si="8"/>
-        <v>12854.566357114854</v>
+        <v>51572.918262664949</v>
       </c>
     </row>
     <row r="167" spans="2:13">
       <c r="B167" s="1"/>
       <c r="C167" s="28">
-        <v>1</v>
+        <v>0.99512</v>
       </c>
       <c r="D167" s="22">
         <v>0.375</v>
       </c>
       <c r="E167" s="22">
-        <v>0</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F167" s="25">
-        <v>10.319000000000001</v>
+        <v>11.452999999999999</v>
       </c>
       <c r="G167" s="22">
-        <v>170000</v>
+        <v>250000</v>
       </c>
       <c r="H167" s="22">
-        <v>5010000</v>
-      </c>
-      <c r="I167" s="17"/>
-      <c r="J167" s="16"/>
-      <c r="K167" s="17"/>
-      <c r="M167" s="1"/>
+        <v>6610000</v>
+      </c>
+      <c r="I167" s="17">
+        <f t="shared" si="3"/>
+        <v>4.8799999999999955E-3</v>
+      </c>
+      <c r="J167" s="16">
+        <f t="shared" si="4"/>
+        <v>10.885999999999999</v>
+      </c>
+      <c r="K167" s="32">
+        <f t="shared" si="5"/>
+        <v>3.4153022626751968</v>
+      </c>
+      <c r="L167" s="1">
+        <f t="shared" si="6"/>
+        <v>209.52858889698757</v>
+      </c>
+      <c r="M167" s="1">
+        <f t="shared" si="7"/>
+        <v>12854.566357114854</v>
+      </c>
     </row>
     <row r="168" spans="2:13">
       <c r="B168" s="1"/>
+      <c r="C168" s="28">
+        <v>1</v>
+      </c>
+      <c r="D168" s="22">
+        <v>0.375</v>
+      </c>
+      <c r="E168" s="22">
+        <v>0</v>
+      </c>
+      <c r="F168" s="25">
+        <v>10.319000000000001</v>
+      </c>
+      <c r="G168" s="22">
+        <v>170000</v>
+      </c>
+      <c r="H168" s="22">
+        <v>5010000</v>
+      </c>
+      <c r="I168" s="17"/>
+      <c r="J168" s="16"/>
+      <c r="K168" s="17"/>
+      <c r="M168" s="1"/>
     </row>
     <row r="169" spans="2:13">
       <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="2:13">
+      <c r="B170" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Small changes in calcSys.xlsx
</commit_message>
<xml_diff>
--- a/tools/calcSystProperties.xlsx
+++ b/tools/calcSystProperties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19110" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="15" yWindow="1185" windowWidth="15270" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OC5-visao geral do paper" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="148">
   <si>
     <t>Massa total</t>
   </si>
@@ -452,13 +452,22 @@
   </si>
   <si>
     <t>I roll/pitch (w.r.t own CM)</t>
+  </si>
+  <si>
+    <t>RNA pitch inertia about own CM</t>
+  </si>
+  <si>
+    <t>RNA roll inertia about own CM</t>
+  </si>
+  <si>
+    <t>RNA yaw inertia about own CM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
@@ -467,6 +476,7 @@
     <numFmt numFmtId="168" formatCode="0.000"/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
     <numFmt numFmtId="170" formatCode="0.000%"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -642,7 +652,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -688,12 +698,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -744,12 +752,15 @@
     </xf>
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,21 +1606,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14">
@@ -1640,12 +1654,12 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="L5" s="71" t="s">
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="L5" s="68" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1724,7 +1738,7 @@
       <c r="L8" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="M8" s="72">
+      <c r="M8" s="69">
         <f>M10/M9</f>
         <v>10.661640507864554</v>
       </c>
@@ -1740,19 +1754,19 @@
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="63">
+      <c r="I9" s="61">
         <v>145448.29999999999</v>
       </c>
-      <c r="J9" s="61" t="s">
+      <c r="J9" s="59" t="s">
         <v>120</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="M9" s="72">
+      <c r="M9" s="69">
         <f>PI()/4*(6.5^2*20+3*(12^2*14+24^2*6))</f>
         <v>13556.757698403355</v>
       </c>
@@ -1764,7 +1778,7 @@
       <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f>D23+$D$19*((D9-D22)^2+(D8-D21)^2)+$D$39+D62+$D$58*(($D$9-$D$57-$D$61)^2+(D8-D60)^2)</f>
         <v>11322112687.663284</v>
       </c>
@@ -1784,7 +1798,7 @@
       <c r="L10" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="M10" s="72">
+      <c r="M10" s="69">
         <f>M11+3*M12+M13*M14^2+2*M13*(M14*COS(RADIANS(60)))^2</f>
         <v>144537.27703260185</v>
       </c>
@@ -1796,7 +1810,7 @@
       <c r="C11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <f>D24+$D$19*((D9-D22)^2+(D7-D20)^2)+$D$39+D63+$D$58*(($D$9-$D$57-$D$61)^2+(D7-D59)^2)</f>
         <v>11307426030.279135</v>
       </c>
@@ -1806,7 +1820,7 @@
       <c r="H11" t="s">
         <v>117</v>
       </c>
-      <c r="I11" s="64">
+      <c r="I11" s="62">
         <f>I13+3*I12+3*I14</f>
         <v>380.10490276123983</v>
       </c>
@@ -1816,7 +1830,7 @@
       <c r="L11" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="M11" s="72">
+      <c r="M11" s="69">
         <f>PI()*3.25^4/4</f>
         <v>87.624050565603596</v>
       </c>
@@ -1828,27 +1842,27 @@
       <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <f>D25+$D$19*((D8-D21)^2+(D7-D20))+D64+$D$58*((D8-D60)^2+(D7-D59)^2)</f>
         <v>12283048613.354862</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="65">
+      <c r="I12" s="63">
         <f>PI()*12^2/4</f>
         <v>113.09733552923255</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="59" t="s">
         <v>115</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="M12" s="72">
+      <c r="M12" s="69">
         <f>PI()*6^4/4</f>
         <v>1017.8760197630929</v>
       </c>
@@ -1860,27 +1874,27 @@
       <c r="C13" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D13" s="73">
+      <c r="D13" s="70">
         <f>D27*B2*B3-D6*B3</f>
         <v>1889410.9764372408</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="57" t="s">
         <v>116</v>
       </c>
-      <c r="I13" s="65">
+      <c r="I13" s="63">
         <f>PI()*6.5^2/4</f>
         <v>33.183072403542191</v>
       </c>
-      <c r="J13" s="61" t="s">
+      <c r="J13" s="59" t="s">
         <v>115</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="M13" s="72">
+      <c r="M13" s="69">
         <f>PI()*12^2/4</f>
         <v>113.09733552923255</v>
       </c>
@@ -1889,29 +1903,29 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="70">
+      <c r="D14" s="67">
         <f>D13/B3</f>
         <v>192600.50728208365</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="H14" s="59" t="s">
+      <c r="H14" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="I14" s="65">
+      <c r="I14" s="63">
         <v>2.5432745899999998</v>
       </c>
-      <c r="J14" s="61" t="s">
+      <c r="J14" s="59" t="s">
         <v>115</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="M14" s="72">
+      <c r="M14" s="69">
         <v>28.87</v>
       </c>
       <c r="N14" t="s">
@@ -1922,13 +1936,13 @@
       <c r="C15" s="7"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="61"/>
-    </row>
-    <row r="16" spans="1:14" s="37" customFormat="1" ht="8.25" customHeight="1">
-      <c r="C16" s="38"/>
-      <c r="E16" s="39"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="59"/>
+    </row>
+    <row r="16" spans="1:14" s="35" customFormat="1" ht="8.25" customHeight="1">
+      <c r="C16" s="36"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="3:9">
       <c r="C17" s="7"/>
@@ -2022,7 +2036,7 @@
       <c r="C26" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="58">
+      <c r="D26" s="56">
         <v>20</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -2033,7 +2047,7 @@
       <c r="C27" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="60">
         <v>13917</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -2148,7 +2162,7 @@
       <c r="C38" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D38" s="74">
+      <c r="D38" s="71">
         <f>SUM(K43:K52)</f>
         <v>121699827.35379744</v>
       </c>
@@ -2157,7 +2171,7 @@
       <c r="C39" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D39" s="74">
+      <c r="D39" s="71">
         <f>D33*(D36-D9)^2+D38</f>
         <v>830965815.13161039</v>
       </c>
@@ -2229,7 +2243,7 @@
         <v>603903000000</v>
       </c>
       <c r="G43" s="24">
-        <f>$D$31+C43*$D$37</f>
+        <f t="shared" ref="G43:G53" si="0">$D$31+C43*$D$37</f>
         <v>10</v>
       </c>
       <c r="H43">
@@ -2237,19 +2251,19 @@
         <v>4506.1399999999994</v>
       </c>
       <c r="I43" s="9">
-        <f>(C44-C43)*$D$37</f>
+        <f t="shared" ref="I43:I52" si="1">(C44-C43)*$D$37</f>
         <v>7.76</v>
       </c>
       <c r="J43">
-        <f>I43*H43</f>
+        <f t="shared" ref="J43:J52" si="2">I43*H43</f>
         <v>34967.646399999998</v>
       </c>
       <c r="K43" s="1">
-        <f>I43*(D43*(G43-$D$36)^2+D44*(G44-$D$36)^2)/2</f>
+        <f t="shared" ref="K43:K52" si="3">I43*(D43*(G43-$D$36)^2+D44*(G44-$D$36)^2)/2</f>
         <v>31289254.644519929</v>
       </c>
       <c r="L43">
-        <f>J43*(G44+G43)/2</f>
+        <f t="shared" ref="L43:L52" si="4">J43*(G44+G43)/2</f>
         <v>485350.93203199992</v>
       </c>
     </row>
@@ -2267,7 +2281,7 @@
         <v>517644000000</v>
       </c>
       <c r="G44" s="24">
-        <f>$D$31+C44*$D$37</f>
+        <f t="shared" si="0"/>
         <v>17.759999999999998</v>
       </c>
       <c r="H44">
@@ -2275,19 +2289,19 @@
         <v>4190.0200000000004</v>
       </c>
       <c r="I44" s="9">
-        <f>(C45-C44)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.76</v>
       </c>
       <c r="J44">
-        <f>I44*H44</f>
+        <f t="shared" si="2"/>
         <v>32514.555200000003</v>
       </c>
       <c r="K44" s="1">
-        <f>I44*(D44*(G44-$D$36)^2+D45*(G45-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>16091940.35343617</v>
       </c>
       <c r="L44">
-        <f>J44*(G45+G44)/2</f>
+        <f t="shared" si="4"/>
         <v>703614.97452800011</v>
       </c>
     </row>
@@ -2305,27 +2319,27 @@
         <v>440925000000</v>
       </c>
       <c r="G45" s="24">
-        <f>$D$31+C45*$D$37</f>
+        <f t="shared" si="0"/>
         <v>25.52</v>
       </c>
       <c r="H45">
-        <f t="shared" ref="H45:H52" si="0">(D45+D46)/2</f>
+        <f t="shared" ref="H45:H52" si="5">(D45+D46)/2</f>
         <v>3885.1000000000004</v>
       </c>
       <c r="I45" s="9">
-        <f>(C46-C45)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.759999999999998</v>
       </c>
       <c r="J45">
-        <f>I45*H45</f>
+        <f t="shared" si="2"/>
         <v>30148.375999999997</v>
       </c>
       <c r="K45" s="1">
-        <f>I45*(D45*(G45-$D$36)^2+D46*(G46-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>6491182.317938488</v>
       </c>
       <c r="L45">
-        <f>J45*(G46+G45)/2</f>
+        <f t="shared" si="4"/>
         <v>886362.25439999986</v>
       </c>
     </row>
@@ -2343,27 +2357,27 @@
         <v>373022000000</v>
       </c>
       <c r="G46" s="24">
-        <f>$D$31+C46*$D$37</f>
+        <f t="shared" si="0"/>
         <v>33.28</v>
       </c>
       <c r="H46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3591.38</v>
       </c>
       <c r="I46" s="9">
-        <f>(C47-C46)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.7600000000000025</v>
       </c>
       <c r="J46">
-        <f>I46*H46</f>
+        <f t="shared" si="2"/>
         <v>27869.108800000009</v>
       </c>
       <c r="K46" s="1">
-        <f>I46*(D46*(G46-$D$36)^2+D47*(G47-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>1559703.3366068501</v>
       </c>
       <c r="L46">
-        <f>J46*(G47+G46)/2</f>
+        <f t="shared" si="4"/>
         <v>1035616.0830080003</v>
       </c>
     </row>
@@ -2381,27 +2395,27 @@
         <v>313236000000</v>
       </c>
       <c r="G47" s="24">
-        <f>$D$31+C47*$D$37</f>
+        <f t="shared" si="0"/>
         <v>41.04</v>
       </c>
       <c r="H47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3308.86</v>
       </c>
       <c r="I47" s="9">
-        <f>(C48-C47)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.759999999999998</v>
       </c>
       <c r="J47">
-        <f>I47*H47</f>
+        <f t="shared" si="2"/>
         <v>25676.753599999993</v>
       </c>
       <c r="K47" s="1">
-        <f>I47*(D47*(G47-$D$36)^2+D48*(G48-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>433029.79263560765</v>
       </c>
       <c r="L47">
-        <f>J47*(G48+G47)/2</f>
+        <f t="shared" si="4"/>
         <v>1153399.7717119998</v>
       </c>
     </row>
@@ -2419,27 +2433,27 @@
         <v>260897000000</v>
       </c>
       <c r="G48" s="24">
-        <f>$D$31+C48*$D$37</f>
+        <f t="shared" si="0"/>
         <v>48.8</v>
       </c>
       <c r="H48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3037.5450000000001</v>
       </c>
       <c r="I48" s="9">
-        <f>(C49-C48)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.759999999999998</v>
       </c>
       <c r="J48">
-        <f>I48*H48</f>
+        <f t="shared" si="2"/>
         <v>23571.349199999993</v>
       </c>
       <c r="K48" s="1">
-        <f>I48*(D48*(G48-$D$36)^2+D49*(G49-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>2309498.3709639874</v>
       </c>
       <c r="L48">
-        <f>J48*(G49+G48)/2</f>
+        <f t="shared" si="4"/>
         <v>1241738.6758559996</v>
       </c>
     </row>
@@ -2457,27 +2471,27 @@
         <v>215365000000</v>
       </c>
       <c r="G49" s="24">
-        <f>$D$31+C49*$D$37</f>
+        <f t="shared" si="0"/>
         <v>56.559999999999995</v>
       </c>
       <c r="H49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2777.4349999999999</v>
       </c>
       <c r="I49" s="9">
-        <f>(C50-C49)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.759999999999998</v>
       </c>
       <c r="J49">
-        <f>I49*H49</f>
+        <f t="shared" si="2"/>
         <v>21552.895599999993</v>
       </c>
       <c r="K49" s="1">
-        <f>I49*(D49*(G49-$D$36)^2+D50*(G50-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>6450263.1432590503</v>
       </c>
       <c r="L49">
-        <f>J49*(G50+G49)/2</f>
+        <f t="shared" si="4"/>
         <v>1302657.0100639996</v>
       </c>
     </row>
@@ -2495,27 +2509,27 @@
         <v>176028000000</v>
       </c>
       <c r="G50" s="24">
-        <f>$D$31+C50*$D$37</f>
+        <f t="shared" si="0"/>
         <v>64.319999999999993</v>
       </c>
       <c r="H50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2528.5299999999997</v>
       </c>
       <c r="I50" s="9">
-        <f>(C51-C50)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.760000000000006</v>
       </c>
       <c r="J50">
-        <f>I50*H50</f>
+        <f t="shared" si="2"/>
         <v>19621.392800000012</v>
       </c>
       <c r="K50" s="1">
-        <f>I50*(D50*(G50-$D$36)^2+D51*(G51-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>12179320.976589227</v>
       </c>
       <c r="L50">
-        <f>J50*(G51+G50)/2</f>
+        <f t="shared" si="4"/>
         <v>1338178.9889600007</v>
       </c>
     </row>
@@ -2533,27 +2547,27 @@
         <v>142301000000</v>
       </c>
       <c r="G51" s="24">
-        <f>$D$31+C51*$D$37</f>
+        <f t="shared" si="0"/>
         <v>72.08</v>
       </c>
       <c r="H51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2290.8249999999998</v>
       </c>
       <c r="I51" s="9">
-        <f>(C52-C51)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.759999999999998</v>
       </c>
       <c r="J51">
-        <f>I51*H51</f>
+        <f t="shared" si="2"/>
         <v>17776.801999999992</v>
       </c>
       <c r="K51" s="1">
-        <f>I51*(D51*(G51-$D$36)^2+D52*(G52-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>18883428.326054338</v>
       </c>
       <c r="L51">
-        <f>J51*(G52+G51)/2</f>
+        <f t="shared" si="4"/>
         <v>1350325.8799199995</v>
       </c>
     </row>
@@ -2571,27 +2585,27 @@
         <v>113630000000</v>
       </c>
       <c r="G52" s="24">
-        <f>$D$31+C52*$D$37</f>
+        <f t="shared" si="0"/>
         <v>79.84</v>
       </c>
       <c r="H52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2064.3199999999997</v>
       </c>
       <c r="I52" s="9">
-        <f>(C53-C52)*$D$37</f>
+        <f t="shared" si="1"/>
         <v>7.759999999999998</v>
       </c>
       <c r="J52">
-        <f>I52*H52</f>
+        <f t="shared" si="2"/>
         <v>16019.123199999995</v>
       </c>
       <c r="K52" s="1">
-        <f>I52*(D52*(G52-$D$36)^2+D53*(G53-$D$36)^2)/2</f>
+        <f t="shared" si="3"/>
         <v>26012206.091793783</v>
       </c>
       <c r="L52">
-        <f>J52*(G53+G52)/2</f>
+        <f t="shared" si="4"/>
         <v>1341120.9943039995</v>
       </c>
     </row>
@@ -2609,7 +2623,7 @@
         <v>89488000000</v>
       </c>
       <c r="G53" s="24">
-        <f>$D$31+C53*$D$37</f>
+        <f t="shared" si="0"/>
         <v>87.6</v>
       </c>
       <c r="I53" s="1"/>
@@ -2646,7 +2660,7 @@
       <c r="C58" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="68">
+      <c r="D58" s="66">
         <f>D92+D69</f>
         <v>349606.48991791578</v>
       </c>
@@ -2691,38 +2705,38 @@
       </c>
     </row>
     <row r="62" spans="3:12">
-      <c r="C62" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D62" s="43">
+      <c r="C62" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="D62" s="72">
         <f>D73+D99</f>
         <v>35235759.645324498</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="39" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="63" spans="3:12">
-      <c r="C63" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="43">
-        <f t="shared" ref="D63" si="1">D74+D100</f>
+      <c r="C63" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="72">
+        <f t="shared" ref="D63" si="6">D74+D100</f>
         <v>20526545.746608194</v>
       </c>
-      <c r="E63" s="41" t="s">
+      <c r="E63" s="39" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="64" spans="3:12">
-      <c r="C64" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D64" s="43">
+      <c r="C64" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="D64" s="72">
         <f>D75+D101</f>
         <v>23112723.553578477</v>
       </c>
-      <c r="E64" s="41" t="s">
+      <c r="E64" s="39" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2825,10 +2839,10 @@
       </c>
     </row>
     <row r="76" spans="3:5">
-      <c r="C76" s="33" t="s">
+      <c r="C76" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="49">
+      <c r="D76" s="47">
         <v>0</v>
       </c>
       <c r="E76" s="16" t="s">
@@ -2836,10 +2850,10 @@
       </c>
     </row>
     <row r="77" spans="3:5">
-      <c r="C77" s="33" t="s">
+      <c r="C77" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D77" s="49">
+      <c r="D77" s="47">
         <v>0</v>
       </c>
       <c r="E77" s="16" t="s">
@@ -2847,10 +2861,10 @@
       </c>
     </row>
     <row r="78" spans="3:5">
-      <c r="C78" s="33" t="s">
+      <c r="C78" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D78" s="49">
+      <c r="D78" s="47">
         <f>D68</f>
         <v>2607890</v>
       </c>
@@ -2859,7 +2873,7 @@
       </c>
     </row>
     <row r="79" spans="3:5">
-      <c r="C79" s="33" t="s">
+      <c r="C79" s="32" t="s">
         <v>89</v>
       </c>
       <c r="D79" s="24">
@@ -2871,11 +2885,11 @@
       </c>
     </row>
     <row r="80" spans="3:5">
-      <c r="C80" s="33" t="s">
+      <c r="C80" s="32" t="s">
         <v>90</v>
       </c>
       <c r="D80" s="24">
-        <f t="shared" ref="D80:D81" si="2">D71-D60</f>
+        <f t="shared" ref="D80:D81" si="7">D71-D60</f>
         <v>0</v>
       </c>
       <c r="E80" s="16" t="s">
@@ -2883,11 +2897,11 @@
       </c>
     </row>
     <row r="81" spans="3:5">
-      <c r="C81" s="33" t="s">
+      <c r="C81" s="32" t="s">
         <v>91</v>
       </c>
       <c r="D81" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>-0.20326319087335687</v>
       </c>
       <c r="E81" s="16" t="s">
@@ -2984,31 +2998,31 @@
       <c r="C92" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D92" s="69">
+      <c r="D92" s="73">
         <f>D93+D94</f>
         <v>109606.48991791575</v>
       </c>
     </row>
     <row r="93" spans="3:5">
-      <c r="C93" s="33" t="s">
+      <c r="C93" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D93" s="34">
+      <c r="D93" s="75">
         <f>D111*D113</f>
         <v>52826.489917915751</v>
       </c>
-      <c r="E93" s="35" t="s">
+      <c r="E93" s="33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="94" spans="3:5">
-      <c r="C94" s="33" t="s">
+      <c r="C94" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D94" s="36">
+      <c r="D94" s="34">
         <v>56780</v>
       </c>
-      <c r="E94" s="35" t="s">
+      <c r="E94" s="33" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3016,7 +3030,7 @@
       <c r="C95" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D95" s="44">
+      <c r="D95" s="42">
         <v>115926</v>
       </c>
       <c r="E95" t="s">
@@ -3027,7 +3041,7 @@
       <c r="C96" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D96" s="47">
+      <c r="D96" s="45">
         <f>(D89)*COS(RADIANS(D90))</f>
         <v>-4.9809734904587275</v>
       </c>
@@ -3039,7 +3053,7 @@
       <c r="C97" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D97" s="47">
+      <c r="D97" s="45">
         <v>0</v>
       </c>
       <c r="E97" t="s">
@@ -3050,7 +3064,7 @@
       <c r="C98" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D98" s="47">
+      <c r="D98" s="45">
         <f>D87-D57</f>
         <v>2.3983387137382834</v>
       </c>
@@ -3080,7 +3094,7 @@
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="B101" s="41"/>
+      <c r="B101" s="39"/>
       <c r="C101" s="6" t="s">
         <v>88</v>
       </c>
@@ -3093,16 +3107,16 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="41"/>
-      <c r="B102" s="41"/>
-      <c r="C102" s="33" t="s">
+      <c r="A102" s="39"/>
+      <c r="B102" s="39"/>
+      <c r="C102" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="D102" s="45">
+      <c r="D102" s="43">
         <f>D95+D111*D114</f>
         <v>35214047.452294782</v>
       </c>
-      <c r="E102" s="35" t="s">
+      <c r="E102" s="33" t="s">
         <v>76</v>
       </c>
       <c r="F102" t="s">
@@ -3110,16 +3124,16 @@
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="41"/>
-      <c r="B103" s="41"/>
-      <c r="C103" s="33" t="s">
+      <c r="A103" s="39"/>
+      <c r="B103" s="39"/>
+      <c r="C103" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D103" s="45">
+      <c r="D103" s="43">
         <f>D111*D114/2</f>
         <v>17549060.726147391</v>
       </c>
-      <c r="E103" s="35" t="s">
+      <c r="E103" s="33" t="s">
         <v>76</v>
       </c>
       <c r="F103" t="s">
@@ -3127,23 +3141,23 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="41"/>
-      <c r="B104" s="41"/>
-      <c r="C104" s="33" t="s">
+      <c r="A104" s="39"/>
+      <c r="B104" s="39"/>
+      <c r="C104" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D104" s="45">
+      <c r="D104" s="43">
         <f>D111*D114/2</f>
         <v>17549060.726147391</v>
       </c>
-      <c r="E104" s="35" t="s">
+      <c r="E104" s="33" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="41"/>
-      <c r="B105" s="41"/>
-      <c r="C105" s="33" t="s">
+      <c r="A105" s="39"/>
+      <c r="B105" s="39"/>
+      <c r="C105" s="32" t="s">
         <v>89</v>
       </c>
       <c r="D105" s="9">
@@ -3152,23 +3166,23 @@
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="41"/>
-      <c r="B106" s="41"/>
-      <c r="C106" s="33" t="s">
+      <c r="A106" s="39"/>
+      <c r="B106" s="39"/>
+      <c r="C106" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D106" s="46">
+      <c r="D106" s="44">
         <f>D97-D60</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="41"/>
-      <c r="B107" s="41"/>
-      <c r="C107" s="33" t="s">
+      <c r="A107" s="39"/>
+      <c r="B107" s="39"/>
+      <c r="C107" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D107" s="46">
+      <c r="D107" s="44">
         <f>D98-D61</f>
         <v>0.44507552286492658</v>
       </c>
@@ -3177,10 +3191,10 @@
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="41"/>
-      <c r="B108" s="41"/>
-      <c r="C108" s="33"/>
-      <c r="D108" s="46"/>
+      <c r="A108" s="39"/>
+      <c r="B108" s="39"/>
+      <c r="C108" s="32"/>
+      <c r="D108" s="44"/>
     </row>
     <row r="109" spans="1:6">
       <c r="C109" s="6"/>
@@ -3211,12 +3225,16 @@
       <c r="E112" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="F112">
+        <f>D111*D113</f>
+        <v>52826.489917915751</v>
+      </c>
     </row>
     <row r="113" spans="2:13">
       <c r="C113" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D113" s="31">
+      <c r="D113" s="74">
         <f>SUM(K120:K167)</f>
         <v>17608.829972638585</v>
       </c>
@@ -3229,7 +3247,7 @@
       <c r="C114" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="2">
         <f>SUM(M120:M167)</f>
         <v>11699373.817431593</v>
       </c>
@@ -3241,7 +3259,7 @@
       <c r="C115" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="2">
         <f>SUM(L120:L167)</f>
         <v>361473.08643987949</v>
       </c>
@@ -3330,23 +3348,23 @@
         <v>18113600000</v>
       </c>
       <c r="I120" s="17">
-        <f t="shared" ref="I120:I167" si="3">C121-C120</f>
+        <f t="shared" ref="I120:I167" si="8">C121-C120</f>
         <v>3.2499999999999999E-3</v>
       </c>
       <c r="J120" s="16">
-        <f t="shared" ref="J120:J167" si="4">(F120+F121)/2</f>
+        <f t="shared" ref="J120:J167" si="9">(F120+F121)/2</f>
         <v>678.93499999999995</v>
       </c>
-      <c r="K120" s="32">
-        <f t="shared" ref="K120:K167" si="5">I120*$D$112*J120*(1+$D$118)</f>
+      <c r="K120" s="31">
+        <f t="shared" ref="K120:K167" si="10">I120*$D$112*J120*(1+$D$118)</f>
         <v>141.85758188355001</v>
       </c>
       <c r="L120" s="1">
-        <f t="shared" ref="L120:L167" si="6">K120*((C120+C121)/2*$D$112)</f>
+        <f t="shared" ref="L120:L167" si="11">K120*((C120+C121)/2*$D$112)</f>
         <v>14.176892089487279</v>
       </c>
       <c r="M120" s="1">
-        <f t="shared" ref="M120:M167" si="7">K120*((C120+C121)/2*$D$112)^2</f>
+        <f t="shared" ref="M120:M167" si="12">K120*((C120+C121)/2*$D$112)^2</f>
         <v>1.4168031531931351</v>
       </c>
     </row>
@@ -3370,23 +3388,23 @@
         <v>18113600000</v>
       </c>
       <c r="I121" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.626E-2</v>
       </c>
       <c r="J121" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>726.149</v>
       </c>
-      <c r="K121" s="32">
-        <f t="shared" si="5"/>
+      <c r="K121" s="31">
+        <f t="shared" si="10"/>
         <v>759.07952776881359</v>
       </c>
       <c r="L121" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>531.25698909955952</v>
       </c>
       <c r="M121" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>371.81082896110877</v>
       </c>
     </row>
@@ -3410,23 +3428,23 @@
         <v>19558600000</v>
       </c>
       <c r="I122" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6260000000000004E-2</v>
       </c>
       <c r="J122" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>756.95650000000001</v>
       </c>
-      <c r="K122" s="32">
-        <f t="shared" si="5"/>
+      <c r="K122" s="31">
+        <f t="shared" si="10"/>
         <v>791.28413391953188</v>
       </c>
       <c r="L122" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1345.0722478844557</v>
       </c>
       <c r="M122" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2286.4345112888709</v>
       </c>
     </row>
@@ -3451,23 +3469,23 @@
         <v>19497800000</v>
       </c>
       <c r="I123" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J123" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>740.29600000000005</v>
       </c>
-      <c r="K123" s="32">
-        <f t="shared" si="5"/>
+      <c r="K123" s="31">
+        <f t="shared" si="10"/>
         <v>773.8680878017343</v>
       </c>
       <c r="L123" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2089.3277568515123</v>
       </c>
       <c r="M123" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5640.8715443355559</v>
       </c>
     </row>
@@ -3492,23 +3510,23 @@
         <v>19788800000</v>
       </c>
       <c r="I124" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6260000000000004E-2</v>
       </c>
       <c r="J124" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>666.26900000000001</v>
       </c>
-      <c r="K124" s="32">
-        <f t="shared" si="5"/>
+      <c r="K124" s="31">
+        <f t="shared" si="10"/>
         <v>696.48399693038175</v>
       </c>
       <c r="L124" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2576.8793512029038</v>
       </c>
       <c r="M124" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>9534.0412987545533</v>
       </c>
     </row>
@@ -3533,23 +3551,23 @@
         <v>14858500000</v>
       </c>
       <c r="I125" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J125" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>521.38549999999998</v>
       </c>
-      <c r="K125" s="32">
-        <f t="shared" si="5"/>
+      <c r="K125" s="31">
+        <f t="shared" si="10"/>
         <v>545.03009592453714</v>
       </c>
       <c r="L125" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2561.5487957290175</v>
       </c>
       <c r="M125" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>12038.843876631108</v>
       </c>
     </row>
@@ -3574,23 +3592,23 @@
         <v>10220600000</v>
       </c>
       <c r="I126" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J126" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>437.16449999999998</v>
       </c>
-      <c r="K126" s="32">
-        <f t="shared" si="5"/>
+      <c r="K126" s="31">
+        <f t="shared" si="10"/>
         <v>456.98971177718278</v>
       </c>
       <c r="L126" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2604.7590989818218</v>
       </c>
       <c r="M126" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>14846.658007558568</v>
       </c>
     </row>
@@ -3615,23 +3633,23 @@
         <v>9144700000</v>
       </c>
       <c r="I127" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J127" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>412.346</v>
       </c>
-      <c r="K127" s="32">
-        <f t="shared" si="5"/>
+      <c r="K127" s="31">
+        <f t="shared" si="10"/>
         <v>431.04570405985436</v>
       </c>
       <c r="L127" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2887.9243185172527</v>
       </c>
       <c r="M127" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>19348.544228445069</v>
       </c>
     </row>
@@ -3656,23 +3674,23 @@
         <v>8063160000</v>
       </c>
       <c r="I128" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6280000000000003E-2</v>
       </c>
       <c r="J128" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>391.35</v>
       </c>
-      <c r="K128" s="32">
-        <f t="shared" si="5"/>
+      <c r="K128" s="31">
+        <f t="shared" si="10"/>
         <v>409.60073999592015</v>
       </c>
       <c r="L128" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3154.0956822756834</v>
       </c>
       <c r="M128" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>24287.845703230905</v>
       </c>
     </row>
@@ -3697,23 +3715,23 @@
         <v>6884440000</v>
       </c>
       <c r="I129" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6240000000000004E-2</v>
       </c>
       <c r="J129" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>390.85849999999999</v>
       </c>
-      <c r="K129" s="32">
-        <f t="shared" si="5"/>
+      <c r="K129" s="31">
+        <f t="shared" si="10"/>
         <v>408.08119263646574</v>
       </c>
       <c r="L129" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>3550.4716488202698</v>
       </c>
       <c r="M129" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>30890.541285754116</v>
       </c>
     </row>
@@ -3738,23 +3756,23 @@
         <v>7009180000</v>
       </c>
       <c r="I130" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J130" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>412.988</v>
       </c>
-      <c r="K130" s="32">
-        <f t="shared" si="5"/>
+      <c r="K130" s="31">
+        <f t="shared" si="10"/>
         <v>431.71681846864317</v>
       </c>
       <c r="L130" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4187.558161445776</v>
       </c>
       <c r="M130" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>40618.392903228509</v>
       </c>
     </row>
@@ -3779,23 +3797,23 @@
         <v>7167680000</v>
       </c>
       <c r="I131" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J131" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>421.57050000000004</v>
       </c>
-      <c r="K131" s="32">
-        <f t="shared" si="5"/>
+      <c r="K131" s="31">
+        <f t="shared" si="10"/>
         <v>440.68853095062116</v>
       </c>
       <c r="L131" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4715.2659228095272</v>
       </c>
       <c r="M131" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>50452.26086289969</v>
       </c>
     </row>
@@ -3820,23 +3838,23 @@
         <v>7271660000</v>
       </c>
       <c r="I132" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J132" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>411.50299999999999</v>
       </c>
-      <c r="K132" s="32">
-        <f t="shared" si="5"/>
+      <c r="K132" s="31">
+        <f t="shared" si="10"/>
         <v>430.16447439223913</v>
       </c>
       <c r="L132" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5032.8211109153435</v>
       </c>
       <c r="M132" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>58882.799120642892</v>
       </c>
     </row>
@@ -3861,23 +3879,23 @@
         <v>7081700000</v>
       </c>
       <c r="I133" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6280000000000017E-2</v>
       </c>
       <c r="J133" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>393.803</v>
       </c>
-      <c r="K133" s="32">
-        <f t="shared" si="5"/>
+      <c r="K133" s="31">
+        <f t="shared" si="10"/>
         <v>412.16813648297813</v>
       </c>
       <c r="L133" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5234.6857747036383</v>
       </c>
       <c r="M133" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>66482.419999043981</v>
       </c>
     </row>
@@ -3902,23 +3920,23 @@
         <v>6244530000</v>
       </c>
       <c r="I134" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6240000000000004E-2</v>
       </c>
       <c r="J134" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>367.12099999999998</v>
       </c>
-      <c r="K134" s="32">
-        <f t="shared" si="5"/>
+      <c r="K134" s="31">
+        <f t="shared" si="10"/>
         <v>383.29772928538574</v>
       </c>
       <c r="L134" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5251.3149619036813</v>
       </c>
       <c r="M134" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>71944.879194891924</v>
       </c>
     </row>
@@ -3943,23 +3961,23 @@
         <v>5048960000</v>
       </c>
       <c r="I135" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999997E-2</v>
       </c>
       <c r="J135" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>351.14949999999999</v>
       </c>
-      <c r="K135" s="32">
-        <f t="shared" si="5"/>
+      <c r="K135" s="31">
+        <f t="shared" si="10"/>
         <v>367.07397054358677</v>
       </c>
       <c r="L135" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5395.8882570186788</v>
       </c>
       <c r="M135" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>79318.100488345182</v>
       </c>
     </row>
@@ -3984,23 +4002,23 @@
         <v>4948490000</v>
       </c>
       <c r="I136" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999969E-2</v>
       </c>
       <c r="J136" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>348.00749999999999</v>
       </c>
-      <c r="K136" s="32">
-        <f t="shared" si="5"/>
+      <c r="K136" s="31">
+        <f t="shared" si="10"/>
         <v>363.78948226879731</v>
       </c>
       <c r="L136" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>5711.3930105650834</v>
       </c>
       <c r="M136" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>89667.271075828859</v>
       </c>
     </row>
@@ -4025,23 +4043,23 @@
         <v>4808020000</v>
       </c>
       <c r="I137" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2540000000000013E-2</v>
       </c>
       <c r="J137" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>342.93550000000005</v>
       </c>
-      <c r="K137" s="32">
-        <f t="shared" si="5"/>
+      <c r="K137" s="31">
+        <f t="shared" si="10"/>
         <v>717.41588273567925</v>
       </c>
       <c r="L137" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>12339.782756136157</v>
       </c>
       <c r="M137" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>212248.21213602385</v>
       </c>
     </row>
@@ -4066,23 +4084,23 @@
         <v>4501400000</v>
       </c>
       <c r="I138" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2509999999999983E-2</v>
       </c>
       <c r="J138" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>334.66849999999999</v>
       </c>
-      <c r="K138" s="32">
-        <f t="shared" si="5"/>
+      <c r="K138" s="31">
+        <f t="shared" si="10"/>
         <v>699.47597216489305</v>
       </c>
       <c r="L138" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>13430.363597219035</v>
       </c>
       <c r="M138" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>257871.14001249071</v>
       </c>
     </row>
@@ -4107,23 +4125,23 @@
         <v>4244070000</v>
       </c>
       <c r="I139" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2520000000000049E-2</v>
       </c>
       <c r="J139" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>325.99700000000001</v>
       </c>
-      <c r="K139" s="32">
-        <f t="shared" si="5"/>
+      <c r="K139" s="31">
+        <f t="shared" si="10"/>
         <v>681.5616321555226</v>
       </c>
       <c r="L139" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>14449.297438954085</v>
       </c>
       <c r="M139" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>306329.15150910954</v>
       </c>
     </row>
@@ -4148,23 +4166,23 @@
         <v>3995280000</v>
       </c>
       <c r="I140" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J140" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>317.90499999999997</v>
       </c>
-      <c r="K140" s="32">
-        <f t="shared" si="5"/>
+      <c r="K140" s="31">
+        <f t="shared" si="10"/>
         <v>664.64369509658388</v>
       </c>
       <c r="L140" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>15419.906533601472</v>
       </c>
       <c r="M140" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>357745.84075525287</v>
       </c>
     </row>
@@ -4189,23 +4207,23 @@
         <v>3750760000</v>
       </c>
       <c r="I141" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J141" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>304.27699999999999</v>
       </c>
-      <c r="K141" s="32">
-        <f t="shared" si="5"/>
+      <c r="K141" s="31">
+        <f t="shared" si="10"/>
         <v>636.15164785990555</v>
       </c>
       <c r="L141" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>16031.174202465107</v>
       </c>
       <c r="M141" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>403989.43738392927</v>
       </c>
     </row>
@@ -4230,23 +4248,23 @@
         <v>3447140000</v>
       </c>
       <c r="I142" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2530000000000003E-2</v>
       </c>
       <c r="J142" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>290.92700000000002</v>
       </c>
-      <c r="K142" s="32">
-        <f t="shared" si="5"/>
+      <c r="K142" s="31">
+        <f t="shared" si="10"/>
         <v>608.42785089198856</v>
       </c>
       <c r="L142" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>16549.558489953437</v>
       </c>
       <c r="M142" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>450156.72081883694</v>
       </c>
     </row>
@@ -4271,23 +4289,23 @@
         <v>3139070000</v>
       </c>
       <c r="I143" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2509999999999983E-2</v>
       </c>
       <c r="J143" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>275.23149999999998</v>
       </c>
-      <c r="K143" s="32">
-        <f t="shared" si="5"/>
+      <c r="K143" s="31">
+        <f t="shared" si="10"/>
         <v>575.24930201946631</v>
       </c>
       <c r="L143" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>16797.571557989191</v>
       </c>
       <c r="M143" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>490497.61426085007</v>
       </c>
     </row>
@@ -4312,23 +4330,23 @@
         <v>2734240000</v>
       </c>
       <c r="I144" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2520000000000049E-2</v>
       </c>
       <c r="J144" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>258.27499999999998</v>
       </c>
-      <c r="K144" s="32">
-        <f t="shared" si="5"/>
+      <c r="K144" s="31">
+        <f t="shared" si="10"/>
         <v>539.97530819292081</v>
       </c>
       <c r="L144" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>16847.326811174604</v>
       </c>
       <c r="M144" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>525639.62902747362</v>
       </c>
     </row>
@@ -4353,23 +4371,23 @@
         <v>2554870000</v>
       </c>
       <c r="I145" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J145" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>247.4365</v>
       </c>
-      <c r="K145" s="32">
-        <f t="shared" si="5"/>
+      <c r="K145" s="31">
+        <f t="shared" si="10"/>
         <v>517.31526607560716</v>
       </c>
       <c r="L145" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>17174.949604152731</v>
       </c>
       <c r="M145" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>570211.07484980742</v>
       </c>
     </row>
@@ -4394,23 +4412,23 @@
         <v>2334030000</v>
       </c>
       <c r="I146" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J146" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>231.15199999999999</v>
       </c>
-      <c r="K146" s="32">
-        <f t="shared" si="5"/>
+      <c r="K146" s="31">
+        <f t="shared" si="10"/>
         <v>483.26927669890551</v>
       </c>
       <c r="L146" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>17011.146197500209</v>
       </c>
       <c r="M146" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>598794.72771247511</v>
       </c>
     </row>
@@ -4435,23 +4453,23 @@
         <v>1828730000</v>
       </c>
       <c r="I147" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2529999999999948E-2</v>
       </c>
       <c r="J147" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>210.46550000000002</v>
       </c>
-      <c r="K147" s="32">
-        <f t="shared" si="5"/>
+      <c r="K147" s="31">
+        <f t="shared" si="10"/>
         <v>440.15533742797203</v>
       </c>
       <c r="L147" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>16373.966718727312</v>
       </c>
       <c r="M147" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>609118.56180742825</v>
       </c>
     </row>
@@ -4476,23 +4494,23 @@
         <v>1584100000</v>
       </c>
       <c r="I148" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2510000000000039E-2</v>
       </c>
       <c r="J148" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>189.8485</v>
       </c>
-      <c r="K148" s="32">
-        <f t="shared" si="5"/>
+      <c r="K148" s="31">
+        <f t="shared" si="10"/>
         <v>396.79403380224591</v>
       </c>
       <c r="L148" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>15554.487818616813</v>
       </c>
       <c r="M148" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>609742.26094356505</v>
       </c>
     </row>
@@ -4517,23 +4535,23 @@
         <v>1323360000</v>
       </c>
       <c r="I149" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J149" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>172.249</v>
       </c>
-      <c r="K149" s="32">
-        <f t="shared" si="5"/>
+      <c r="K149" s="31">
+        <f t="shared" si="10"/>
         <v>360.12082803570718</v>
       </c>
       <c r="L149" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>14837.006924737381</v>
       </c>
       <c r="M149" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>611285.8722597342</v>
       </c>
     </row>
@@ -4558,23 +4576,23 @@
         <v>1183680000</v>
       </c>
       <c r="I150" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J150" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>159.7525</v>
       </c>
-      <c r="K150" s="32">
-        <f t="shared" si="5"/>
+      <c r="K150" s="31">
+        <f t="shared" si="10"/>
         <v>333.99440682253197</v>
       </c>
       <c r="L150" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>14428.578414397791</v>
       </c>
       <c r="M150" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>623315.45321668941</v>
       </c>
     </row>
@@ -4599,23 +4617,23 @@
         <v>1020160000</v>
       </c>
       <c r="I151" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J151" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>146.673</v>
       </c>
-      <c r="K151" s="32">
-        <f t="shared" si="5"/>
+      <c r="K151" s="31">
+        <f t="shared" si="10"/>
         <v>306.64910803825438</v>
       </c>
       <c r="L151" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>13860.55194929342</v>
       </c>
       <c r="M151" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>626497.50253014057</v>
       </c>
     </row>
@@ -4640,23 +4658,23 @@
         <v>797810000</v>
       </c>
       <c r="I152" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2540000000000013E-2</v>
       </c>
       <c r="J152" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>134.245</v>
       </c>
-      <c r="K152" s="32">
-        <f t="shared" si="5"/>
+      <c r="K152" s="31">
+        <f t="shared" si="10"/>
         <v>280.83851096737214</v>
       </c>
       <c r="L152" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>13255.756050114429</v>
       </c>
       <c r="M152" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>625680.10297049279</v>
       </c>
     </row>
@@ -4681,23 +4699,23 @@
         <v>709610000</v>
       </c>
       <c r="I153" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2499999999999973E-2</v>
       </c>
       <c r="J153" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>118.40950000000001</v>
       </c>
-      <c r="K153" s="32">
-        <f t="shared" si="5"/>
+      <c r="K153" s="31">
+        <f t="shared" si="10"/>
         <v>247.40638414634984</v>
       </c>
       <c r="L153" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>12172.546254926661</v>
       </c>
       <c r="M153" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>598896.76185833861</v>
       </c>
     </row>
@@ -4722,23 +4740,23 @@
         <v>518190000</v>
       </c>
       <c r="I154" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J154" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>103.02</v>
       </c>
-      <c r="K154" s="32">
-        <f t="shared" si="5"/>
+      <c r="K154" s="31">
+        <f t="shared" si="10"/>
         <v>215.38382054025598</v>
       </c>
       <c r="L154" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>11027.647303984695</v>
       </c>
       <c r="M154" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>564615.32141107018</v>
       </c>
     </row>
@@ -4763,23 +4781,23 @@
         <v>454870000</v>
       </c>
       <c r="I155" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>3.2519999999999993E-2</v>
       </c>
       <c r="J155" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>94.512</v>
       </c>
-      <c r="K155" s="32">
-        <f t="shared" si="5"/>
+      <c r="K155" s="31">
+        <f t="shared" si="10"/>
         <v>197.59615265871358</v>
       </c>
       <c r="L155" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>10512.107417597457</v>
       </c>
       <c r="M155" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>559243.69413188798</v>
       </c>
     </row>
@@ -4804,23 +4822,23 @@
         <v>395120000</v>
       </c>
       <c r="I156" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6260000000000052E-2</v>
       </c>
       <c r="J156" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>86.624500000000012</v>
       </c>
-      <c r="K156" s="32">
-        <f t="shared" si="5"/>
+      <c r="K156" s="31">
+        <f t="shared" si="10"/>
         <v>90.552881782127116</v>
       </c>
       <c r="L156" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4953.2376530738547</v>
       </c>
       <c r="M156" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>270941.82719506894</v>
       </c>
     </row>
@@ -4845,23 +4863,23 @@
         <v>353720000</v>
       </c>
       <c r="I157" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6259999999999941E-2</v>
       </c>
       <c r="J157" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>77.953500000000005</v>
       </c>
-      <c r="K157" s="32">
-        <f t="shared" si="5"/>
+      <c r="K157" s="31">
+        <f t="shared" si="10"/>
         <v>81.488655865292117</v>
       </c>
       <c r="L157" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4538.912834934139</v>
       </c>
       <c r="M157" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>252817.14987649728</v>
       </c>
     </row>
@@ -4886,23 +4904,23 @@
         <v>304730000</v>
       </c>
       <c r="I158" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.6260000000000052E-2</v>
       </c>
       <c r="J158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>70.838999999999999</v>
       </c>
-      <c r="K158" s="32">
-        <f t="shared" si="5"/>
+      <c r="K158" s="31">
+        <f t="shared" si="10"/>
         <v>74.051516517429846</v>
       </c>
       <c r="L158" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>4198.7154326745331</v>
       </c>
       <c r="M158" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>238066.85012898859</v>
       </c>
     </row>
@@ -4927,23 +4945,23 @@
         <v>281420000</v>
       </c>
       <c r="I159" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1299999999999706E-3</v>
       </c>
       <c r="J159" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>67.518000000000001</v>
       </c>
-      <c r="K159" s="32">
-        <f t="shared" si="5"/>
+      <c r="K159" s="31">
+        <f t="shared" si="10"/>
         <v>35.289955336917473</v>
       </c>
       <c r="L159" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>2027.4050226845934</v>
       </c>
       <c r="M159" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>116474.25129231552</v>
       </c>
     </row>
@@ -4968,23 +4986,23 @@
         <v>261710000</v>
       </c>
       <c r="I160" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1499999999999906E-3</v>
       </c>
       <c r="J160" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>62.802</v>
       </c>
-      <c r="K160" s="32">
-        <f t="shared" si="5"/>
+      <c r="K160" s="31">
+        <f t="shared" si="10"/>
         <v>32.905771465931956</v>
       </c>
       <c r="L160" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1906.9068142452052</v>
       </c>
       <c r="M160" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>110506.25577885416</v>
       </c>
     </row>
@@ -5009,23 +5027,23 @@
         <v>158810000</v>
       </c>
       <c r="I161" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1100000000000616E-3</v>
       </c>
       <c r="J161" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>57.627000000000002</v>
       </c>
-      <c r="K161" s="32">
-        <f t="shared" si="5"/>
+      <c r="K161" s="31">
+        <f t="shared" si="10"/>
         <v>30.046082773511031</v>
       </c>
       <c r="L161" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1756.2092371899689</v>
       </c>
       <c r="M161" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>102651.3475330801</v>
       </c>
     </row>
@@ -5050,23 +5068,23 @@
         <v>137880000</v>
       </c>
       <c r="I162" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1299999999999706E-3</v>
       </c>
       <c r="J162" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>54.198999999999998</v>
       </c>
-      <c r="K162" s="32">
-        <f t="shared" si="5"/>
+      <c r="K162" s="31">
+        <f t="shared" si="10"/>
         <v>28.328450032666698</v>
       </c>
       <c r="L162" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1669.9593674018236</v>
       </c>
       <c r="M162" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>98443.941887299181</v>
       </c>
     </row>
@@ -5091,23 +5109,23 @@
         <v>118790000</v>
       </c>
       <c r="I163" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1299999999999706E-3</v>
       </c>
       <c r="J163" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>50.798999999999999</v>
       </c>
-      <c r="K163" s="32">
-        <f t="shared" si="5"/>
+      <c r="K163" s="31">
+        <f t="shared" si="10"/>
         <v>26.551355803786706</v>
       </c>
       <c r="L163" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1578.4753810211498</v>
       </c>
       <c r="M163" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>93840.199607980787</v>
       </c>
     </row>
@@ -5132,23 +5150,23 @@
         <v>101630000</v>
       </c>
       <c r="I164" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1299999999999706E-3</v>
       </c>
       <c r="J164" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>47.465999999999994</v>
       </c>
-      <c r="K164" s="32">
-        <f t="shared" si="5"/>
+      <c r="K164" s="31">
+        <f t="shared" si="10"/>
         <v>24.80928078471111</v>
       </c>
       <c r="L164" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1487.3137160457466</v>
       </c>
       <c r="M164" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>89164.297390718028</v>
       </c>
     </row>
@@ -5173,23 +5191,23 @@
         <v>85070000</v>
       </c>
       <c r="I165" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1300000000000816E-3</v>
       </c>
       <c r="J165" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>43.743499999999997</v>
       </c>
-      <c r="K165" s="32">
-        <f t="shared" si="5"/>
+      <c r="K165" s="31">
+        <f t="shared" si="10"/>
         <v>22.86362394147443</v>
       </c>
       <c r="L165" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1382.103495104436</v>
       </c>
       <c r="M165" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>83548.00079241996</v>
       </c>
     </row>
@@ -5214,23 +5232,23 @@
         <v>64260000</v>
       </c>
       <c r="I166" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>8.1299999999999706E-3</v>
       </c>
       <c r="J166" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>26.561</v>
       </c>
-      <c r="K166" s="32">
-        <f t="shared" si="5"/>
+      <c r="K166" s="31">
+        <f t="shared" si="10"/>
         <v>13.88276465096515</v>
       </c>
       <c r="L166" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>846.15287425147937</v>
       </c>
       <c r="M166" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>51572.918262664949</v>
       </c>
     </row>
@@ -5255,23 +5273,23 @@
         <v>6610000</v>
       </c>
       <c r="I167" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>4.8799999999999955E-3</v>
       </c>
       <c r="J167" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>10.885999999999999</v>
       </c>
-      <c r="K167" s="32">
-        <f t="shared" si="5"/>
+      <c r="K167" s="31">
+        <f t="shared" si="10"/>
         <v>3.4153022626751968</v>
       </c>
       <c r="L167" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>209.52858889698757</v>
       </c>
       <c r="M167" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>12854.566357114854</v>
       </c>
     </row>
@@ -5338,10 +5356,10 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="53" t="s">
         <v>108</v>
       </c>
     </row>
@@ -5472,9 +5490,9 @@
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="3:12" s="37" customFormat="1">
-      <c r="C11" s="38"/>
-      <c r="E11" s="39"/>
+    <row r="11" spans="3:12" s="35" customFormat="1">
+      <c r="C11" s="36"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="3:12">
       <c r="C12" s="7"/>
@@ -5491,7 +5509,7 @@
       <c r="C14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="49">
         <v>12919000</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -5604,7 +5622,7 @@
       <c r="C26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="50">
+      <c r="D26" s="48">
         <f>493500</f>
         <v>493500</v>
       </c>
@@ -5649,7 +5667,7 @@
       <c r="C30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="48">
+      <c r="D30" s="46">
         <f>D25-D24</f>
         <v>78.2</v>
       </c>
@@ -5734,38 +5752,38 @@
       </c>
     </row>
     <row r="39" spans="3:6">
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="43">
+      <c r="D39" s="41">
         <f>D50+D76</f>
         <v>111003326</v>
       </c>
-      <c r="E39" s="41" t="s">
+      <c r="E39" s="39" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="3:6">
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="43">
+      <c r="D40" s="41">
         <f t="shared" ref="D40" si="1">D51+D77</f>
         <v>114471551.91183783</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E40" s="39" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="3:6">
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="43">
+      <c r="D41" s="41">
         <f>D52+D78</f>
         <v>114471551.91183783</v>
       </c>
-      <c r="E41" s="41" t="s">
+      <c r="E41" s="39" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5871,7 +5889,7 @@
       </c>
     </row>
     <row r="53" spans="3:5">
-      <c r="C53" s="33" t="s">
+      <c r="C53" s="32" t="s">
         <v>82</v>
       </c>
       <c r="D53" s="22">
@@ -5882,7 +5900,7 @@
       </c>
     </row>
     <row r="54" spans="3:5">
-      <c r="C54" s="33" t="s">
+      <c r="C54" s="32" t="s">
         <v>83</v>
       </c>
       <c r="D54" s="22">
@@ -5893,7 +5911,7 @@
       </c>
     </row>
     <row r="55" spans="3:5">
-      <c r="C55" s="33" t="s">
+      <c r="C55" s="32" t="s">
         <v>84</v>
       </c>
       <c r="D55" s="22">
@@ -5904,7 +5922,7 @@
       </c>
     </row>
     <row r="56" spans="3:5">
-      <c r="C56" s="33" t="s">
+      <c r="C56" s="32" t="s">
         <v>89</v>
       </c>
       <c r="D56" s="24">
@@ -5916,7 +5934,7 @@
       </c>
     </row>
     <row r="57" spans="3:5">
-      <c r="C57" s="33" t="s">
+      <c r="C57" s="32" t="s">
         <v>90</v>
       </c>
       <c r="D57" s="24">
@@ -5928,7 +5946,7 @@
       </c>
     </row>
     <row r="58" spans="3:5">
-      <c r="C58" s="33" t="s">
+      <c r="C58" s="32" t="s">
         <v>91</v>
       </c>
       <c r="D58" s="24">
@@ -6029,31 +6047,31 @@
       <c r="C69" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D69" s="40">
+      <c r="D69" s="38">
         <f>D70+D71</f>
         <v>66999</v>
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="C70" s="33" t="s">
+      <c r="C70" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D70" s="52">
+      <c r="D70" s="50">
         <f>D88*D90</f>
         <v>66999</v>
       </c>
-      <c r="E70" s="35" t="s">
+      <c r="E70" s="33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="C71" s="33" t="s">
+      <c r="C71" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D71" s="53">
+      <c r="D71" s="51">
         <v>0</v>
       </c>
-      <c r="E71" s="35" t="s">
+      <c r="E71" s="33" t="s">
         <v>8</v>
       </c>
       <c r="F71" t="s">
@@ -6064,7 +6082,7 @@
       <c r="C72" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D72" s="44">
+      <c r="D72" s="42">
         <v>115926</v>
       </c>
       <c r="E72" t="s">
@@ -6075,7 +6093,7 @@
       <c r="C73" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D73" s="47">
+      <c r="D73" s="45">
         <f>(D66)*COS(RADIANS(D67))</f>
         <v>10.6</v>
       </c>
@@ -6087,7 +6105,7 @@
       <c r="C74" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D74" s="47">
+      <c r="D74" s="45">
         <v>0</v>
       </c>
       <c r="E74" t="s">
@@ -6098,7 +6116,7 @@
       <c r="C75" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D75" s="47">
+      <c r="D75" s="45">
         <f>D64-D34</f>
         <v>1.7999999999999972</v>
       </c>
@@ -6128,7 +6146,7 @@
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="B78" s="41"/>
+      <c r="B78" s="39"/>
       <c r="C78" s="6" t="s">
         <v>88</v>
       </c>
@@ -6141,16 +6159,16 @@
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="41"/>
-      <c r="B79" s="41"/>
-      <c r="C79" s="33" t="s">
+      <c r="A79" s="39"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="D79" s="45">
+      <c r="D79" s="43">
         <f>D72+D88*D91</f>
         <v>44590326</v>
       </c>
-      <c r="E79" s="35" t="s">
+      <c r="E79" s="33" t="s">
         <v>76</v>
       </c>
       <c r="F79" t="s">
@@ -6158,16 +6176,16 @@
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="41"/>
-      <c r="B80" s="41"/>
-      <c r="C80" s="33" t="s">
+      <c r="A80" s="39"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="D80" s="45">
+      <c r="D80" s="43">
         <f>D88*D91/2</f>
         <v>22237200</v>
       </c>
-      <c r="E80" s="35" t="s">
+      <c r="E80" s="33" t="s">
         <v>76</v>
       </c>
       <c r="F80" t="s">
@@ -6175,23 +6193,23 @@
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="41"/>
-      <c r="B81" s="41"/>
-      <c r="C81" s="33" t="s">
+      <c r="A81" s="39"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D81" s="45">
+      <c r="D81" s="43">
         <f>D88*D91/2</f>
         <v>22237200</v>
       </c>
-      <c r="E81" s="35" t="s">
+      <c r="E81" s="33" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="41"/>
-      <c r="B82" s="41"/>
-      <c r="C82" s="33" t="s">
+      <c r="A82" s="39"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="32" t="s">
         <v>89</v>
       </c>
       <c r="D82" s="9">
@@ -6200,23 +6218,23 @@
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="41"/>
-      <c r="B83" s="41"/>
-      <c r="C83" s="33" t="s">
+      <c r="A83" s="39"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D83" s="46">
+      <c r="D83" s="44">
         <f>D74-D37</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="41"/>
-      <c r="B84" s="41"/>
-      <c r="C84" s="33" t="s">
+      <c r="A84" s="39"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D84" s="46">
+      <c r="D84" s="44">
         <f>D75-D38</f>
         <v>-2.4424906541753444E-15</v>
       </c>
@@ -6225,10 +6243,10 @@
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="41"/>
-      <c r="B85" s="41"/>
-      <c r="C85" s="33"/>
-      <c r="D85" s="46"/>
+      <c r="A85" s="39"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="44"/>
     </row>
     <row r="86" spans="1:6">
       <c r="C86" s="6"/>
@@ -6264,7 +6282,7 @@
       <c r="C90" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D90" s="54">
+      <c r="D90" s="52">
         <v>22333</v>
       </c>
       <c r="E90" s="4" t="s">
@@ -6321,8 +6339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>